<commit_message>
changed many files but accomplished 0 tasks
</commit_message>
<xml_diff>
--- a/Documentation/Working Hours.xlsx
+++ b/Documentation/Working Hours.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
-  <workbookPr filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="162913"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
   <si>
     <t>Working Hours</t>
   </si>
@@ -79,6 +79,18 @@
   </si>
   <si>
     <t>servlets,finance</t>
+  </si>
+  <si>
+    <t>Grand Total hours</t>
+  </si>
+  <si>
+    <t>Total Tasks completed</t>
+  </si>
+  <si>
+    <t>Documentation</t>
+  </si>
+  <si>
+    <t>Database, Servlets(Session), GUI</t>
   </si>
   <si>
     <t>enroll funciton</t>
@@ -93,11 +105,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -114,7 +126,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -136,6 +148,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -167,36 +185,54 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -259,7 +295,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -294,7 +330,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -471,357 +507,714 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="81" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="1.85546875" customWidth="1"/>
-    <col min="7" max="7" width="60.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="50" customWidth="1"/>
-    <col min="9" max="9" width="46.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="4"/>
+    <col min="3" max="3" width="6.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="1.85546875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="64" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="50" style="4" customWidth="1"/>
+    <col min="9" max="9" width="46.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="2" t="s">
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="2" t="s">
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="4"/>
-      <c r="B2" s="9" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="G2" s="9" t="s">
+      <c r="E2" s="3"/>
+      <c r="G2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="H2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="I2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="5"/>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="4">
+      <c r="J2" s="3"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
         <v>43735</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="3">
         <v>9</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5">
+      <c r="C3" s="3"/>
+      <c r="D3" s="3">
         <v>8</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="3">
         <f>B3+C3+D3</f>
         <v>17</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5" t="s">
+      <c r="H3" s="3"/>
+      <c r="I3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="5">
+      <c r="J3" s="3">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="4">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
         <v>43736</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="3">
         <v>5</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5">
+      <c r="C4" s="3"/>
+      <c r="D4" s="3">
         <v>0</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="3">
         <f t="shared" ref="E4:E6" si="0">B4+C4+D4</f>
         <v>5</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5" t="s">
+      <c r="H4" s="3"/>
+      <c r="I4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="J4" s="5">
+      <c r="J4" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="4">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
         <v>43737</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="3">
         <v>9</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5">
+      <c r="C5" s="3"/>
+      <c r="D5" s="3">
         <v>0</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5" t="s">
+      <c r="H5" s="3"/>
+      <c r="I5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="J5" s="5">
+      <c r="J5" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="4">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
         <v>43738</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="3">
         <v>0</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5">
+      <c r="C6" s="3"/>
+      <c r="D6" s="3">
         <v>3</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="3">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5" t="s">
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="J6" s="5">
+      <c r="J6" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="8" customFormat="1">
-      <c r="A7" s="7"/>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="4">
+    <row r="7" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="11"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
         <v>43739</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="3">
         <v>8</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5">
+      <c r="C8" s="3"/>
+      <c r="D8" s="3">
         <v>0.5</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="3">
         <f>B8+C8+D8</f>
         <v>8.5</v>
       </c>
-      <c r="F8" s="6"/>
-      <c r="G8" s="5" t="s">
+      <c r="G8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5" t="s">
+      <c r="H8" s="3"/>
+      <c r="I8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J8" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" s="4">
+      <c r="J8" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
         <v>43740</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="3">
         <v>7</v>
       </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5">
+      <c r="C9" s="3"/>
+      <c r="D9" s="3">
         <v>7</v>
       </c>
-      <c r="E9" s="5">
-        <f t="shared" ref="E9:E14" si="1">B9+C9+D9</f>
+      <c r="E9" s="3">
+        <f t="shared" ref="E9:E15" si="1">B9+C9+D9</f>
         <v>14</v>
       </c>
-      <c r="F9" s="6"/>
-      <c r="G9" s="5" t="s">
+      <c r="G9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5" t="s">
+      <c r="H9" s="3"/>
+      <c r="I9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="J9" s="5">
+      <c r="J9" s="3">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
-      <c r="A10" s="4">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
         <v>43741</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="3">
         <v>5</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5">
+      <c r="C10" s="3"/>
+      <c r="D10" s="3">
         <v>2</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="3">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="F10" s="6"/>
-      <c r="G10" s="5" t="s">
+      <c r="G10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5" t="s">
+      <c r="H10" s="3"/>
+      <c r="I10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="J10" s="5">
+      <c r="J10" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
-      <c r="A11" s="4">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
         <v>43742</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="3">
         <v>4</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5">
+      <c r="C11" s="3"/>
+      <c r="D11" s="3">
         <v>4</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="3">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="F11" s="6"/>
-      <c r="G11" s="5" t="s">
+      <c r="G11" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5" t="s">
+      <c r="H11" s="3"/>
+      <c r="I11" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="J11" s="5">
+      <c r="J11" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>43743</v>
+      </c>
+      <c r="B12" s="14">
+        <v>7</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3">
+        <v>1</v>
+      </c>
+      <c r="E12" s="3">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="G12" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J12" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>43744</v>
+      </c>
+      <c r="B13" s="14">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="A12" s="4">
-        <v>43743</v>
-      </c>
-      <c r="B12" s="5">
-        <v>7</v>
-      </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5">
-        <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="F12" s="6"/>
-      <c r="G12" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
-      <c r="A13" s="4">
-        <v>43744</v>
-      </c>
-      <c r="B13" s="5">
-        <v>3</v>
-      </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5">
+      <c r="C13" s="3"/>
+      <c r="D13" s="3">
+        <v>0</v>
+      </c>
+      <c r="E13" s="3">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="F13" s="6"/>
-      <c r="G13" s="5" t="s">
+      <c r="G13" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J13" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>43745</v>
+      </c>
+      <c r="B14" s="14">
+        <v>13</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3">
+        <v>8</v>
+      </c>
+      <c r="E14" s="3">
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5">
+      <c r="G14" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J14" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>43746</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" s="4">
-        <v>43745</v>
-      </c>
-      <c r="B14" s="5">
-        <v>13</v>
-      </c>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5">
+      <c r="E15" s="3">
         <f t="shared" si="1"/>
-        <v>13</v>
-      </c>
-      <c r="F14" s="6"/>
-      <c r="G14" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5">
-        <v>5</v>
+        <v>1</v>
+      </c>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>43747</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>43748</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>43749</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>43750</v>
+      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>43751</v>
+      </c>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>43752</v>
+      </c>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>43753</v>
+      </c>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>43754</v>
+      </c>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>43755</v>
+      </c>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>43756</v>
+      </c>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>43757</v>
+      </c>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>43758</v>
+      </c>
+      <c r="B27" s="16"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="15">
+        <v>43759</v>
+      </c>
+      <c r="B28" s="16"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="16"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="16"/>
+      <c r="I28" s="16"/>
+      <c r="J28" s="16"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="15">
+        <v>43760</v>
+      </c>
+      <c r="B29" s="16"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="16"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="16"/>
+      <c r="I29" s="16"/>
+      <c r="J29" s="16"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="15">
+        <v>43761</v>
+      </c>
+      <c r="B30" s="16"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="16"/>
+      <c r="G30" s="16"/>
+      <c r="H30" s="16"/>
+      <c r="I30" s="16"/>
+      <c r="J30" s="16"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="15">
+        <v>43762</v>
+      </c>
+      <c r="B31" s="16"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="16"/>
+      <c r="G31" s="16"/>
+      <c r="H31" s="16"/>
+      <c r="I31" s="16"/>
+      <c r="J31" s="16"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="15">
+        <v>43763</v>
+      </c>
+      <c r="B32" s="16"/>
+      <c r="C32" s="16"/>
+      <c r="D32" s="16"/>
+      <c r="E32" s="16"/>
+      <c r="G32" s="16"/>
+      <c r="H32" s="16"/>
+      <c r="I32" s="16"/>
+      <c r="J32" s="16"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="15">
+        <v>43764</v>
+      </c>
+      <c r="B33" s="16"/>
+      <c r="C33" s="16"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="16"/>
+      <c r="G33" s="16"/>
+      <c r="H33" s="16"/>
+      <c r="I33" s="16"/>
+      <c r="J33" s="16"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="15">
+        <v>43765</v>
+      </c>
+      <c r="B34" s="16"/>
+      <c r="C34" s="16"/>
+      <c r="D34" s="16"/>
+      <c r="E34" s="16"/>
+      <c r="G34" s="16"/>
+      <c r="H34" s="16"/>
+      <c r="I34" s="16"/>
+      <c r="J34" s="16"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="15">
+        <v>43766</v>
+      </c>
+      <c r="B35" s="16"/>
+      <c r="C35" s="16"/>
+      <c r="D35" s="16"/>
+      <c r="E35" s="16"/>
+      <c r="G35" s="16"/>
+      <c r="H35" s="16"/>
+      <c r="I35" s="16"/>
+      <c r="J35" s="16"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="15">
+        <v>43767</v>
+      </c>
+      <c r="B36" s="16"/>
+      <c r="C36" s="16"/>
+      <c r="D36" s="16"/>
+      <c r="E36" s="16"/>
+      <c r="G36" s="16"/>
+      <c r="H36" s="16"/>
+      <c r="I36" s="16"/>
+      <c r="J36" s="16"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="15">
+        <v>43768</v>
+      </c>
+      <c r="B37" s="16"/>
+      <c r="C37" s="16"/>
+      <c r="D37" s="16"/>
+      <c r="E37" s="16"/>
+      <c r="G37" s="16"/>
+      <c r="H37" s="16"/>
+      <c r="I37" s="16"/>
+      <c r="J37" s="16"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="15">
+        <v>43769</v>
+      </c>
+      <c r="B38" s="16"/>
+      <c r="C38" s="16"/>
+      <c r="D38" s="16"/>
+      <c r="E38" s="16"/>
+      <c r="G38" s="16"/>
+      <c r="H38" s="16"/>
+      <c r="I38" s="16"/>
+      <c r="J38" s="16"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B41" s="4">
+        <f>SUM(B3:B28)</f>
+        <v>70</v>
+      </c>
+      <c r="D41" s="4">
+        <f>SUM(D3:D28)</f>
+        <v>34.5</v>
+      </c>
+      <c r="E41" s="4">
+        <f>SUM(E3:E28)</f>
+        <v>104.5</v>
+      </c>
+      <c r="I41" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J41" s="4">
+        <f>SUM(J3:J28)</f>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added CSS in editSubject Servlet
</commit_message>
<xml_diff>
--- a/Documentation/Working Hours.xlsx
+++ b/Documentation/Working Hours.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
   <si>
     <t>Working Hours</t>
   </si>
@@ -100,6 +100,27 @@
   </si>
   <si>
     <t>adv enroll, save timetable, session management, distimetable</t>
+  </si>
+  <si>
+    <t>Thursday, September 26, 2019</t>
+  </si>
+  <si>
+    <t>Fixed navbar, fixed google recaptcha, fixed modal box and added splash screen</t>
+  </si>
+  <si>
+    <t>Sidebar button and Query for Subject table</t>
+  </si>
+  <si>
+    <t>Added dispSubject, editSubject and addSubject Servlets</t>
+  </si>
+  <si>
+    <t>Added deltSubject Servlet</t>
+  </si>
+  <si>
+    <t>Accordion Side menu</t>
+  </si>
+  <si>
+    <t>Added CSS in editSubject Servlet</t>
   </si>
 </sst>
 </file>
@@ -185,7 +206,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -223,16 +244,19 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -515,22 +539,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J41"/>
+  <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="81" workbookViewId="0">
-      <selection activeCell="H40" sqref="H40"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="81" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.28515625" style="9" customWidth="1"/>
     <col min="2" max="2" width="9.140625" style="4"/>
     <col min="3" max="3" width="6.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.42578125" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.5703125" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="1.85546875" style="4" customWidth="1"/>
     <col min="7" max="7" width="64" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="50" style="4" customWidth="1"/>
+    <col min="8" max="8" width="81" style="4" customWidth="1"/>
     <col min="9" max="9" width="46.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="19.42578125" style="4" bestFit="1" customWidth="1"/>
     <col min="11" max="16384" width="9.140625" style="4"/>
@@ -540,19 +564,19 @@
       <c r="A1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
       <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
@@ -581,348 +605,385 @@
       <c r="J2" s="3"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>43735</v>
-      </c>
-      <c r="B3" s="3">
-        <v>9</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3">
-        <v>8</v>
-      </c>
-      <c r="E3" s="3">
-        <f>B3+C3+D3</f>
-        <v>17</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J3" s="3">
+      <c r="A3" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="17">
+        <v>5</v>
+      </c>
+      <c r="D3" s="6"/>
+      <c r="E3" s="15">
+        <f>(B3+C3+D3)</f>
+        <v>5</v>
+      </c>
+      <c r="G3" s="5"/>
+      <c r="H3" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" s="6"/>
+      <c r="J3" s="15">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <v>43736</v>
+        <v>43735</v>
       </c>
       <c r="B4" s="3">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E4" s="3">
-        <f t="shared" ref="E4:E6" si="0">B4+C4+D4</f>
-        <v>5</v>
+        <f>B4+C4+D4</f>
+        <v>17</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H4" s="3"/>
       <c r="I4" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="J4" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>43737</v>
+        <v>43736</v>
       </c>
       <c r="B5" s="3">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3">
         <v>0</v>
       </c>
       <c r="E5" s="3">
-        <f t="shared" si="0"/>
-        <v>9</v>
+        <f t="shared" ref="E5:E7" si="0">B5+C5+D5</f>
+        <v>5</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="3" t="s">
         <v>13</v>
       </c>
       <c r="J5" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>43738</v>
+        <v>43737</v>
       </c>
       <c r="B6" s="3">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E6" s="3">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="G6" s="3"/>
+        <v>9</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="H6" s="3"/>
       <c r="I6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J6" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>43738</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3">
+        <v>3</v>
+      </c>
+      <c r="E7" s="3">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F7" s="4"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="J6" s="3">
+      <c r="J7" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-    </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>43739</v>
-      </c>
-      <c r="B8" s="3">
-        <v>8</v>
-      </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="E8" s="3">
-        <f>B8+C8+D8</f>
-        <v>8.5</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J8" s="3">
-        <v>1</v>
-      </c>
+      <c r="A8" s="11"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
-        <v>43740</v>
+        <v>43739</v>
       </c>
       <c r="B9" s="3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3">
-        <v>7</v>
+        <v>0.5</v>
       </c>
       <c r="E9" s="3">
-        <f t="shared" ref="E9:E15" si="1">B9+C9+D9</f>
-        <v>14</v>
+        <f>B9+C9+D9</f>
+        <v>8.5</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>18</v>
       </c>
       <c r="H9" s="3"/>
       <c r="I9" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="J9" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
-        <v>43741</v>
+        <v>43740</v>
       </c>
       <c r="B10" s="3">
+        <v>7</v>
+      </c>
+      <c r="C10" s="3">
         <v>5</v>
       </c>
-      <c r="C10" s="3"/>
       <c r="D10" s="3">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E10" s="3">
-        <f t="shared" si="1"/>
-        <v>7</v>
+        <f t="shared" ref="E10:E16" si="1">B10+C10+D10</f>
+        <v>19</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H10" s="3"/>
+      <c r="H10" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="I10" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J10" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
-        <v>43742</v>
+        <v>43741</v>
       </c>
       <c r="B11" s="3">
-        <v>4</v>
-      </c>
-      <c r="C11" s="3"/>
+        <v>5</v>
+      </c>
+      <c r="C11" s="3">
+        <v>3</v>
+      </c>
       <c r="D11" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E11" s="3">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H11" s="3"/>
+        <v>18</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="I11" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J11" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
-        <v>43743</v>
-      </c>
-      <c r="B12" s="14">
-        <v>7</v>
-      </c>
-      <c r="C12" s="3"/>
+        <v>43742</v>
+      </c>
+      <c r="B12" s="3">
+        <v>4</v>
+      </c>
+      <c r="C12" s="3">
+        <v>1</v>
+      </c>
       <c r="D12" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E12" s="3">
         <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="G12" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="H12" s="3"/>
+        <v>9</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>31</v>
+      </c>
       <c r="I12" s="3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="J12" s="3">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
-        <v>43744</v>
-      </c>
-      <c r="B13" s="14">
-        <v>3</v>
+        <v>43743</v>
+      </c>
+      <c r="B13" s="13">
+        <v>7</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" s="3">
         <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="G13" s="16" t="s">
-        <v>25</v>
+        <v>8</v>
+      </c>
+      <c r="G13" s="15" t="s">
+        <v>24</v>
       </c>
       <c r="H13" s="3"/>
       <c r="I13" s="3" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="J13" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <v>43745</v>
-      </c>
-      <c r="B14" s="14">
-        <v>13</v>
+        <v>43744</v>
+      </c>
+      <c r="B14" s="13">
+        <v>3</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E14" s="3">
         <f t="shared" si="1"/>
-        <v>21</v>
-      </c>
-      <c r="G14" s="16" t="s">
-        <v>26</v>
+        <v>3</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>25</v>
       </c>
       <c r="H14" s="3"/>
       <c r="I14" s="3" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="J14" s="3">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <v>43746</v>
-      </c>
-      <c r="B15" s="3"/>
+        <v>43745</v>
+      </c>
+      <c r="B15" s="13">
+        <v>13</v>
+      </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E15" s="3">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="G15" s="3"/>
+        <v>21</v>
+      </c>
+      <c r="G15" s="15" t="s">
+        <v>26</v>
+      </c>
       <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
+      <c r="I15" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J15" s="3">
+        <v>3</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <v>43747</v>
+        <v>43746</v>
       </c>
       <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
+      <c r="C16" s="3">
+        <v>4</v>
+      </c>
+      <c r="D16" s="3">
+        <v>1</v>
+      </c>
+      <c r="E16" s="3">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
       <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
+      <c r="H16" s="3" t="s">
+        <v>32</v>
+      </c>
       <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
+      <c r="J16" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <v>43748</v>
+        <v>43747</v>
       </c>
       <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
+      <c r="C17" s="3">
+        <v>3</v>
+      </c>
       <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
+      <c r="E17" s="3">
+        <f>(B17+C17+D17)</f>
+        <v>3</v>
+      </c>
       <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
+      <c r="H17" s="3" t="s">
+        <v>33</v>
+      </c>
       <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
+      <c r="J17" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <v>43749</v>
+        <v>43748</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -935,7 +996,7 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <v>43750</v>
+        <v>43749</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -948,7 +1009,7 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <v>43751</v>
+        <v>43750</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -961,7 +1022,7 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <v>43752</v>
+        <v>43751</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -974,7 +1035,7 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
-        <v>43753</v>
+        <v>43752</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -987,7 +1048,7 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
-        <v>43754</v>
+        <v>43753</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -1000,7 +1061,7 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
-        <v>43755</v>
+        <v>43754</v>
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -1013,7 +1074,7 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
-        <v>43756</v>
+        <v>43755</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -1026,7 +1087,7 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
-        <v>43757</v>
+        <v>43756</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -1039,182 +1100,199 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
-        <v>43758</v>
-      </c>
-      <c r="B27" s="16"/>
-      <c r="C27" s="16"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="16"/>
+        <v>43757</v>
+      </c>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="15">
+      <c r="A28" s="2">
+        <v>43758</v>
+      </c>
+      <c r="B28" s="15"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="14">
         <v>43759</v>
       </c>
-      <c r="B28" s="16"/>
-      <c r="C28" s="16"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="16"/>
-      <c r="G28" s="16"/>
-      <c r="H28" s="16"/>
-      <c r="I28" s="16"/>
-      <c r="J28" s="16"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="15">
+      <c r="B29" s="15"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="15"/>
+      <c r="I29" s="15"/>
+      <c r="J29" s="15"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="14">
         <v>43760</v>
       </c>
-      <c r="B29" s="16"/>
-      <c r="C29" s="16"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="16"/>
-      <c r="G29" s="16"/>
-      <c r="H29" s="16"/>
-      <c r="I29" s="16"/>
-      <c r="J29" s="16"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="15">
+      <c r="B30" s="15"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="15"/>
+      <c r="G30" s="15"/>
+      <c r="H30" s="15"/>
+      <c r="I30" s="15"/>
+      <c r="J30" s="15"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="14">
         <v>43761</v>
       </c>
-      <c r="B30" s="16"/>
-      <c r="C30" s="16"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="16"/>
-      <c r="G30" s="16"/>
-      <c r="H30" s="16"/>
-      <c r="I30" s="16"/>
-      <c r="J30" s="16"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="15">
+      <c r="B31" s="15"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="15"/>
+      <c r="I31" s="15"/>
+      <c r="J31" s="15"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="14">
         <v>43762</v>
       </c>
-      <c r="B31" s="16"/>
-      <c r="C31" s="16"/>
-      <c r="D31" s="16"/>
-      <c r="E31" s="16"/>
-      <c r="G31" s="16"/>
-      <c r="H31" s="16"/>
-      <c r="I31" s="16"/>
-      <c r="J31" s="16"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="15">
+      <c r="B32" s="15"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="15"/>
+      <c r="G32" s="15"/>
+      <c r="H32" s="15"/>
+      <c r="I32" s="15"/>
+      <c r="J32" s="15"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="14">
         <v>43763</v>
       </c>
-      <c r="B32" s="16"/>
-      <c r="C32" s="16"/>
-      <c r="D32" s="16"/>
-      <c r="E32" s="16"/>
-      <c r="G32" s="16"/>
-      <c r="H32" s="16"/>
-      <c r="I32" s="16"/>
-      <c r="J32" s="16"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="15">
+      <c r="B33" s="15"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="15"/>
+      <c r="G33" s="15"/>
+      <c r="H33" s="15"/>
+      <c r="I33" s="15"/>
+      <c r="J33" s="15"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="14">
         <v>43764</v>
       </c>
-      <c r="B33" s="16"/>
-      <c r="C33" s="16"/>
-      <c r="D33" s="16"/>
-      <c r="E33" s="16"/>
-      <c r="G33" s="16"/>
-      <c r="H33" s="16"/>
-      <c r="I33" s="16"/>
-      <c r="J33" s="16"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="15">
+      <c r="B34" s="15"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="15"/>
+      <c r="E34" s="15"/>
+      <c r="G34" s="15"/>
+      <c r="H34" s="15"/>
+      <c r="I34" s="15"/>
+      <c r="J34" s="15"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="14">
         <v>43765</v>
       </c>
-      <c r="B34" s="16"/>
-      <c r="C34" s="16"/>
-      <c r="D34" s="16"/>
-      <c r="E34" s="16"/>
-      <c r="G34" s="16"/>
-      <c r="H34" s="16"/>
-      <c r="I34" s="16"/>
-      <c r="J34" s="16"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="15">
+      <c r="B35" s="15"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="15"/>
+      <c r="G35" s="15"/>
+      <c r="H35" s="15"/>
+      <c r="I35" s="15"/>
+      <c r="J35" s="15"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="14">
         <v>43766</v>
       </c>
-      <c r="B35" s="16"/>
-      <c r="C35" s="16"/>
-      <c r="D35" s="16"/>
-      <c r="E35" s="16"/>
-      <c r="G35" s="16"/>
-      <c r="H35" s="16"/>
-      <c r="I35" s="16"/>
-      <c r="J35" s="16"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="15">
+      <c r="B36" s="15"/>
+      <c r="C36" s="15"/>
+      <c r="D36" s="15"/>
+      <c r="E36" s="15"/>
+      <c r="G36" s="15"/>
+      <c r="H36" s="15"/>
+      <c r="I36" s="15"/>
+      <c r="J36" s="15"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="14">
         <v>43767</v>
       </c>
-      <c r="B36" s="16"/>
-      <c r="C36" s="16"/>
-      <c r="D36" s="16"/>
-      <c r="E36" s="16"/>
-      <c r="G36" s="16"/>
-      <c r="H36" s="16"/>
-      <c r="I36" s="16"/>
-      <c r="J36" s="16"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="15">
+      <c r="B37" s="15"/>
+      <c r="C37" s="15"/>
+      <c r="D37" s="15"/>
+      <c r="E37" s="15"/>
+      <c r="G37" s="15"/>
+      <c r="H37" s="15"/>
+      <c r="I37" s="15"/>
+      <c r="J37" s="15"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="14">
         <v>43768</v>
       </c>
-      <c r="B37" s="16"/>
-      <c r="C37" s="16"/>
-      <c r="D37" s="16"/>
-      <c r="E37" s="16"/>
-      <c r="G37" s="16"/>
-      <c r="H37" s="16"/>
-      <c r="I37" s="16"/>
-      <c r="J37" s="16"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="15">
+      <c r="B38" s="15"/>
+      <c r="C38" s="15"/>
+      <c r="D38" s="15"/>
+      <c r="E38" s="15"/>
+      <c r="G38" s="15"/>
+      <c r="H38" s="15"/>
+      <c r="I38" s="15"/>
+      <c r="J38" s="15"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="14">
         <v>43769</v>
       </c>
-      <c r="B38" s="16"/>
-      <c r="C38" s="16"/>
-      <c r="D38" s="16"/>
-      <c r="E38" s="16"/>
-      <c r="G38" s="16"/>
-      <c r="H38" s="16"/>
-      <c r="I38" s="16"/>
-      <c r="J38" s="16"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="9" t="s">
+      <c r="B39" s="15"/>
+      <c r="C39" s="15"/>
+      <c r="D39" s="15"/>
+      <c r="E39" s="15"/>
+      <c r="G39" s="15"/>
+      <c r="H39" s="15"/>
+      <c r="I39" s="15"/>
+      <c r="J39" s="15"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B41" s="4">
-        <f>SUM(B3:B28)</f>
+      <c r="B42" s="4">
+        <f>SUM(B4:B29)</f>
         <v>70</v>
       </c>
-      <c r="D41" s="4">
-        <f>SUM(D3:D28)</f>
+      <c r="C42" s="4">
+        <f>SUM(C3:C29)</f>
+        <v>21</v>
+      </c>
+      <c r="D42" s="4">
+        <f>SUM(D4:D29)</f>
         <v>34.5</v>
       </c>
-      <c r="E41" s="4">
-        <f>SUM(E3:E28)</f>
-        <v>104.5</v>
-      </c>
-      <c r="I41" s="4" t="s">
+      <c r="E42" s="4">
+        <f>SUM(E4:E29)</f>
+        <v>120.5</v>
+      </c>
+      <c r="I42" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="J41" s="4">
-        <f>SUM(J3:J28)</f>
-        <v>25</v>
+      <c r="J42" s="4">
+        <f>SUM(J4:J29)</f>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1223,6 +1301,6 @@
     <mergeCell ref="G1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed image in navbar, added css in editStudent, editFaculty, editTimetable Servlets
</commit_message>
<xml_diff>
--- a/Documentation/Working Hours.xlsx
+++ b/Documentation/Working Hours.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
   <si>
     <t>Working Hours</t>
   </si>
@@ -133,6 +133,9 @@
   </si>
   <si>
     <t>Error Finding, Testing, Documentation</t>
+  </si>
+  <si>
+    <t>Fixed image in navbar, added css in editStudent, editFaculty, editTimetable Servlets</t>
   </si>
 </sst>
 </file>
@@ -274,17 +277,17 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -568,7 +571,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="81" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D4" zoomScale="81" workbookViewId="0">
       <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
@@ -578,33 +581,33 @@
     <col min="2" max="2" width="9.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" style="22" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" style="21" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="1.85546875" style="3" customWidth="1"/>
     <col min="7" max="7" width="64" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="80.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="82.140625" style="3" customWidth="1"/>
     <col min="9" max="9" width="46.28515625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="19.42578125" style="22" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.42578125" style="21" bestFit="1" customWidth="1"/>
     <col min="11" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="20" t="s">
+      <c r="B1" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="21"/>
-      <c r="G1" s="18" t="s">
+      <c r="F1" s="20"/>
+      <c r="G1" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
       <c r="J1" s="17" t="s">
         <v>7</v>
       </c>
@@ -1160,16 +1163,22 @@
         <v>43755</v>
       </c>
       <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
+      <c r="C25" s="2">
+        <v>1.5</v>
+      </c>
       <c r="D25" s="2"/>
       <c r="E25" s="14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
+      <c r="H25" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="I25" s="2"/>
-      <c r="J25" s="14"/>
+      <c r="J25" s="14">
+        <v>2</v>
+      </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
@@ -1413,7 +1422,7 @@
       </c>
       <c r="C42" s="3">
         <f>SUM(C3:C29)</f>
-        <v>21</v>
+        <v>22.5</v>
       </c>
       <c r="D42" s="3">
         <f>SUM(D4:D29)</f>
@@ -1421,14 +1430,14 @@
       </c>
       <c r="E42" s="16">
         <f>SUM(E4:E29)</f>
-        <v>126.5</v>
+        <v>128</v>
       </c>
       <c r="I42" s="3" t="s">
         <v>21</v>
       </c>
       <c r="J42" s="16">
         <f>SUM(J4:J29)</f>
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
documentation, deleteStudent Servlet, workhours
</commit_message>
<xml_diff>
--- a/Documentation/Working Hours.xlsx
+++ b/Documentation/Working Hours.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="52">
   <si>
     <t>Working Hours</t>
   </si>
@@ -169,14 +169,21 @@
   </si>
   <si>
     <t>editProfile servlet</t>
+  </si>
+  <si>
+    <t>addStudent</t>
+  </si>
+  <si>
+    <t>addStudent, database, deleteStudent</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="166" formatCode="[$-14009]dddd\,\ d\ mmmm\,\ yyyy;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -260,7 +267,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -286,9 +293,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -325,9 +329,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -336,6 +337,9 @@
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -620,8 +624,8 @@
   <dimension ref="A1:K42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="81" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C31" sqref="C31"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -630,35 +634,35 @@
     <col min="2" max="2" width="9.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" style="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" style="20" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="1.85546875" style="3" customWidth="1"/>
     <col min="7" max="7" width="64" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="82.140625" style="3" customWidth="1"/>
     <col min="9" max="9" width="46.28515625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="19.42578125" style="21" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.42578125" style="20" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="12" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="19" t="s">
+      <c r="B1" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="20"/>
-      <c r="G1" s="25" t="s">
+      <c r="F1" s="19"/>
+      <c r="G1" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="17" t="s">
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="16" t="s">
         <v>7</v>
       </c>
     </row>
@@ -673,7 +677,7 @@
       <c r="D2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="14"/>
+      <c r="E2" s="13"/>
       <c r="G2" s="4" t="s">
         <v>1</v>
       </c>
@@ -683,33 +687,33 @@
       <c r="I2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="14"/>
+      <c r="J2" s="13"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13">
+      <c r="B3" s="12"/>
+      <c r="C3" s="12">
         <v>5</v>
       </c>
-      <c r="D3" s="13"/>
-      <c r="E3" s="14">
+      <c r="D3" s="12"/>
+      <c r="E3" s="13">
         <f>(B3+C3+D3)</f>
         <v>5</v>
       </c>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13" t="s">
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="I3" s="13"/>
-      <c r="J3" s="14">
+      <c r="I3" s="12"/>
+      <c r="J3" s="13">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+      <c r="A4" s="24">
         <v>43735</v>
       </c>
       <c r="B4" s="2">
@@ -721,7 +725,7 @@
       <c r="D4" s="2">
         <v>8</v>
       </c>
-      <c r="E4" s="14">
+      <c r="E4" s="13">
         <f>B4+C4+D4</f>
         <v>17</v>
       </c>
@@ -732,12 +736,12 @@
       <c r="I4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="14">
+      <c r="J4" s="13">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+      <c r="A5" s="24">
         <v>43736</v>
       </c>
       <c r="B5" s="2">
@@ -749,7 +753,7 @@
       <c r="D5" s="2">
         <v>0</v>
       </c>
-      <c r="E5" s="14">
+      <c r="E5" s="13">
         <f t="shared" ref="E5:E7" si="0">B5+C5+D5</f>
         <v>5</v>
       </c>
@@ -760,12 +764,12 @@
       <c r="I5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J5" s="14">
+      <c r="J5" s="13">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+      <c r="A6" s="24">
         <v>43737</v>
       </c>
       <c r="B6" s="2">
@@ -777,7 +781,7 @@
       <c r="D6" s="2">
         <v>0</v>
       </c>
-      <c r="E6" s="14">
+      <c r="E6" s="13">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
@@ -788,12 +792,12 @@
       <c r="I6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J6" s="14">
+      <c r="J6" s="13">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+      <c r="A7" s="24">
         <v>43738</v>
       </c>
       <c r="B7" s="2">
@@ -805,7 +809,7 @@
       <c r="D7" s="2">
         <v>3</v>
       </c>
-      <c r="E7" s="14">
+      <c r="E7" s="13">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
@@ -815,24 +819,24 @@
       <c r="I7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J7" s="14">
+      <c r="J7" s="13">
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
+      <c r="A8" s="24"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
+      <c r="A9" s="24">
         <v>43739</v>
       </c>
       <c r="B9" s="2">
@@ -844,7 +848,7 @@
       <c r="D9" s="2">
         <v>0.5</v>
       </c>
-      <c r="E9" s="14">
+      <c r="E9" s="13">
         <f>B9+C9+D9</f>
         <v>8.5</v>
       </c>
@@ -855,12 +859,12 @@
       <c r="I9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J9" s="14">
+      <c r="J9" s="13">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
+      <c r="A10" s="24">
         <v>43740</v>
       </c>
       <c r="B10" s="2">
@@ -872,7 +876,7 @@
       <c r="D10" s="2">
         <v>7</v>
       </c>
-      <c r="E10" s="14">
+      <c r="E10" s="13">
         <f t="shared" ref="E10:E16" si="1">B10+C10+D10</f>
         <v>19</v>
       </c>
@@ -885,12 +889,12 @@
       <c r="I10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J10" s="14">
+      <c r="J10" s="13">
         <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
+      <c r="A11" s="24">
         <v>43741</v>
       </c>
       <c r="B11" s="2">
@@ -902,7 +906,7 @@
       <c r="D11" s="2">
         <v>2</v>
       </c>
-      <c r="E11" s="14">
+      <c r="E11" s="13">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
@@ -915,12 +919,12 @@
       <c r="I11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J11" s="14">
+      <c r="J11" s="13">
         <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
+      <c r="A12" s="24">
         <v>43742</v>
       </c>
       <c r="B12" s="2">
@@ -932,7 +936,7 @@
       <c r="D12" s="2">
         <v>4</v>
       </c>
-      <c r="E12" s="14">
+      <c r="E12" s="13">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
@@ -945,15 +949,15 @@
       <c r="I12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J12" s="14">
+      <c r="J12" s="13">
         <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
+      <c r="A13" s="24">
         <v>43743</v>
       </c>
-      <c r="B13" s="11">
+      <c r="B13" s="10">
         <v>7</v>
       </c>
       <c r="C13" s="2">
@@ -962,26 +966,26 @@
       <c r="D13" s="2">
         <v>1</v>
       </c>
-      <c r="E13" s="14">
+      <c r="E13" s="13">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="G13" s="13" t="s">
+      <c r="G13" s="12" t="s">
         <v>24</v>
       </c>
       <c r="H13" s="2"/>
       <c r="I13" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="J13" s="14">
+      <c r="J13" s="13">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
+      <c r="A14" s="24">
         <v>43744</v>
       </c>
-      <c r="B14" s="11">
+      <c r="B14" s="10">
         <v>3</v>
       </c>
       <c r="C14" s="2">
@@ -990,26 +994,26 @@
       <c r="D14" s="2">
         <v>0</v>
       </c>
-      <c r="E14" s="14">
+      <c r="E14" s="13">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="G14" s="13" t="s">
+      <c r="G14" s="12" t="s">
         <v>25</v>
       </c>
       <c r="H14" s="2"/>
       <c r="I14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J14" s="14">
+      <c r="J14" s="13">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
+      <c r="A15" s="24">
         <v>43745</v>
       </c>
-      <c r="B15" s="11">
+      <c r="B15" s="10">
         <v>13</v>
       </c>
       <c r="C15" s="2">
@@ -1018,23 +1022,23 @@
       <c r="D15" s="2">
         <v>8</v>
       </c>
-      <c r="E15" s="14">
+      <c r="E15" s="13">
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="G15" s="13" t="s">
+      <c r="G15" s="12" t="s">
         <v>37</v>
       </c>
       <c r="H15" s="2"/>
       <c r="I15" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J15" s="14">
+      <c r="J15" s="13">
         <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
+      <c r="A16" s="24">
         <v>43746</v>
       </c>
       <c r="B16" s="2">
@@ -1046,11 +1050,11 @@
       <c r="D16" s="2">
         <v>1</v>
       </c>
-      <c r="E16" s="14">
+      <c r="E16" s="13">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="G16" s="13" t="s">
+      <c r="G16" s="12" t="s">
         <v>38</v>
       </c>
       <c r="H16" s="2" t="s">
@@ -1059,12 +1063,12 @@
       <c r="I16" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="J16" s="14">
+      <c r="J16" s="13">
         <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
+      <c r="A17" s="24">
         <v>43747</v>
       </c>
       <c r="B17" s="2">
@@ -1076,7 +1080,7 @@
       <c r="D17" s="2">
         <v>2</v>
       </c>
-      <c r="E17" s="14">
+      <c r="E17" s="13">
         <f>(B17+C17+D17)</f>
         <v>12</v>
       </c>
@@ -1089,12 +1093,12 @@
       <c r="I17" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="J17" s="14">
+      <c r="J17" s="13">
         <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
+      <c r="A18" s="24">
         <v>43748</v>
       </c>
       <c r="B18" s="2">
@@ -1104,23 +1108,23 @@
       <c r="D18" s="2">
         <v>3</v>
       </c>
-      <c r="E18" s="14">
+      <c r="E18" s="13">
         <f t="shared" ref="E18:E39" si="2">B18+C18+D18</f>
         <v>11</v>
       </c>
-      <c r="G18" s="13" t="s">
+      <c r="G18" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="H18" s="13"/>
+      <c r="H18" s="12"/>
       <c r="I18" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="J18" s="14">
+      <c r="J18" s="13">
         <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
+      <c r="A19" s="24">
         <v>43749</v>
       </c>
       <c r="B19" s="2">
@@ -1130,22 +1134,22 @@
       <c r="D19" s="2">
         <v>1</v>
       </c>
-      <c r="E19" s="14">
+      <c r="E19" s="13">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="G19" s="13" t="s">
+      <c r="G19" s="12" t="s">
         <v>42</v>
       </c>
       <c r="I19" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="J19" s="14">
+      <c r="J19" s="13">
         <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
+      <c r="A20" s="24">
         <v>43750</v>
       </c>
       <c r="B20" s="2">
@@ -1155,23 +1159,23 @@
       <c r="D20" s="2">
         <v>0</v>
       </c>
-      <c r="E20" s="14">
+      <c r="E20" s="13">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="G20" s="13" t="s">
+      <c r="G20" s="12" t="s">
         <v>40</v>
       </c>
       <c r="H20" s="2"/>
       <c r="I20" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J20" s="14">
+      <c r="J20" s="13">
         <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
+      <c r="A21" s="24">
         <v>43751</v>
       </c>
       <c r="B21" s="2">
@@ -1181,23 +1185,23 @@
       <c r="D21" s="2">
         <v>0</v>
       </c>
-      <c r="E21" s="14">
+      <c r="E21" s="13">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="G21" s="13" t="s">
+      <c r="G21" s="12" t="s">
         <v>39</v>
       </c>
       <c r="H21" s="2"/>
       <c r="I21" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J21" s="14">
+      <c r="J21" s="13">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
+      <c r="A22" s="24">
         <v>43752</v>
       </c>
       <c r="B22" s="2">
@@ -1207,31 +1211,31 @@
       <c r="D22" s="2">
         <v>0</v>
       </c>
-      <c r="E22" s="14">
+      <c r="E22" s="13">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G22" s="13"/>
+      <c r="G22" s="12"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J22" s="14">
+      <c r="J22" s="13">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
+      <c r="A23" s="24">
         <v>43753</v>
       </c>
-      <c r="B23" s="13">
+      <c r="B23" s="12">
         <v>0</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2">
         <v>0</v>
       </c>
-      <c r="E23" s="14">
+      <c r="E23" s="13">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -1240,39 +1244,39 @@
       <c r="I23" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J23" s="14" t="s">
+      <c r="J23" s="13" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
+      <c r="A24" s="24">
         <v>43754</v>
       </c>
-      <c r="B24" s="13">
+      <c r="B24" s="12">
         <v>0</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2">
         <v>0</v>
       </c>
-      <c r="E24" s="14">
+      <c r="E24" s="13">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G24" s="2"/>
-      <c r="H24" s="13"/>
+      <c r="H24" s="12"/>
       <c r="I24" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J24" s="14" t="s">
+      <c r="J24" s="13" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
+      <c r="A25" s="24">
         <v>43755</v>
       </c>
-      <c r="B25" s="13">
+      <c r="B25" s="12">
         <v>0</v>
       </c>
       <c r="C25" s="2">
@@ -1281,7 +1285,7 @@
       <c r="D25" s="2">
         <v>0</v>
       </c>
-      <c r="E25" s="14">
+      <c r="E25" s="13">
         <f t="shared" si="2"/>
         <v>1.5</v>
       </c>
@@ -1292,22 +1296,22 @@
       <c r="I25" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J25" s="14">
+      <c r="J25" s="13">
         <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
+      <c r="A26" s="24">
         <v>43756</v>
       </c>
-      <c r="B26" s="13">
+      <c r="B26" s="12">
         <v>0</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2">
         <v>0</v>
       </c>
-      <c r="E26" s="14">
+      <c r="E26" s="13">
         <f t="shared" ref="E26" si="3">(B26+C26+D26)</f>
         <v>0</v>
       </c>
@@ -1316,22 +1320,22 @@
       <c r="I26" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J26" s="14" t="s">
+      <c r="J26" s="13" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
+      <c r="A27" s="24">
         <v>43757</v>
       </c>
-      <c r="B27" s="13">
+      <c r="B27" s="12">
         <v>0</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2">
         <v>0</v>
       </c>
-      <c r="E27" s="14">
+      <c r="E27" s="13">
         <f t="shared" ref="E27" si="4">B27+C27+D27</f>
         <v>0</v>
       </c>
@@ -1340,233 +1344,241 @@
       <c r="I27" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J27" s="14"/>
+      <c r="J27" s="13"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
+      <c r="A28" s="24">
         <v>43758</v>
       </c>
-      <c r="B28" s="13">
+      <c r="B28" s="12">
         <v>2</v>
       </c>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13">
+      <c r="C28" s="12"/>
+      <c r="D28" s="12">
         <v>1</v>
       </c>
-      <c r="E28" s="14">
+      <c r="E28" s="13">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="G28" s="13" t="s">
+      <c r="G28" s="12" t="s">
         <v>44</v>
       </c>
       <c r="H28" s="2"/>
       <c r="I28" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="J28" s="14">
+      <c r="J28" s="13">
         <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="12">
+      <c r="A29" s="24">
         <v>43759</v>
       </c>
-      <c r="B29" s="13"/>
-      <c r="C29" s="13">
+      <c r="B29" s="12"/>
+      <c r="C29" s="12">
         <v>8.5</v>
       </c>
-      <c r="D29" s="13"/>
-      <c r="E29" s="14">
+      <c r="D29" s="12">
+        <v>3</v>
+      </c>
+      <c r="E29" s="13">
         <f t="shared" si="2"/>
-        <v>8.5</v>
-      </c>
-      <c r="G29" s="13"/>
-      <c r="H29" s="13" t="s">
+        <v>11.5</v>
+      </c>
+      <c r="G29" s="12"/>
+      <c r="H29" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="I29" s="13"/>
-      <c r="J29" s="14">
+      <c r="I29" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="J29" s="13">
         <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="12">
+      <c r="A30" s="24">
         <v>43760</v>
       </c>
-      <c r="B30" s="13"/>
-      <c r="C30" s="13">
+      <c r="B30" s="12"/>
+      <c r="C30" s="12">
         <v>3</v>
       </c>
-      <c r="D30" s="13"/>
-      <c r="E30" s="14">
+      <c r="D30" s="12">
+        <v>5</v>
+      </c>
+      <c r="E30" s="13">
         <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="G30" s="12"/>
+      <c r="H30" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="I30" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="J30" s="13">
         <v>3</v>
       </c>
-      <c r="G30" s="13"/>
-      <c r="H30" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="I30" s="13"/>
-      <c r="J30" s="14">
-        <v>1</v>
-      </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="12">
+      <c r="A31" s="24">
         <v>43761</v>
       </c>
-      <c r="B31" s="13"/>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="14">
+      <c r="B31" s="12"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="13">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G31" s="13"/>
-      <c r="H31" s="13"/>
-      <c r="I31" s="13"/>
-      <c r="J31" s="14"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="12"/>
+      <c r="I31" s="12"/>
+      <c r="J31" s="13"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="12">
+      <c r="A32" s="24">
         <v>43762</v>
       </c>
-      <c r="B32" s="13"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="14">
+      <c r="B32" s="12"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="13">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G32" s="13"/>
-      <c r="H32" s="13"/>
-      <c r="I32" s="13"/>
-      <c r="J32" s="14"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="12"/>
+      <c r="I32" s="12"/>
+      <c r="J32" s="13"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="12">
+      <c r="A33" s="24">
         <v>43763</v>
       </c>
-      <c r="B33" s="13"/>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="14">
+      <c r="B33" s="12"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="13">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G33" s="13"/>
-      <c r="H33" s="13"/>
-      <c r="I33" s="13"/>
-      <c r="J33" s="14"/>
+      <c r="G33" s="12"/>
+      <c r="H33" s="12"/>
+      <c r="I33" s="12"/>
+      <c r="J33" s="13"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="12">
+      <c r="A34" s="24">
         <v>43764</v>
       </c>
-      <c r="B34" s="13"/>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="14">
+      <c r="B34" s="12"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="13">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G34" s="13"/>
-      <c r="H34" s="13"/>
-      <c r="I34" s="13"/>
-      <c r="J34" s="14"/>
+      <c r="G34" s="12"/>
+      <c r="H34" s="12"/>
+      <c r="I34" s="12"/>
+      <c r="J34" s="13"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="12">
+      <c r="A35" s="24">
         <v>43765</v>
       </c>
-      <c r="B35" s="13"/>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="14">
+      <c r="B35" s="12"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="13">
         <f t="shared" ref="E35" si="5">(B35+C35+D35)</f>
         <v>0</v>
       </c>
-      <c r="G35" s="13"/>
-      <c r="H35" s="13"/>
-      <c r="I35" s="13"/>
-      <c r="J35" s="14"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="12"/>
+      <c r="I35" s="12"/>
+      <c r="J35" s="13"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="12">
+      <c r="A36" s="24">
         <v>43766</v>
       </c>
-      <c r="B36" s="13"/>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="14">
+      <c r="B36" s="12"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="13">
         <f t="shared" ref="E36" si="6">B36+C36+D36</f>
         <v>0</v>
       </c>
-      <c r="G36" s="13"/>
-      <c r="H36" s="13"/>
-      <c r="I36" s="13"/>
-      <c r="J36" s="14"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="12"/>
+      <c r="I36" s="12"/>
+      <c r="J36" s="13"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="22">
+      <c r="A37" s="24">
         <v>43767</v>
       </c>
-      <c r="B37" s="23"/>
-      <c r="C37" s="23"/>
-      <c r="D37" s="23"/>
-      <c r="E37" s="23">
+      <c r="B37" s="21"/>
+      <c r="C37" s="21"/>
+      <c r="D37" s="21"/>
+      <c r="E37" s="21">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F37" s="24"/>
-      <c r="G37" s="23"/>
-      <c r="H37" s="23"/>
-      <c r="I37" s="23"/>
-      <c r="J37" s="23"/>
+      <c r="F37" s="22"/>
+      <c r="G37" s="21"/>
+      <c r="H37" s="21"/>
+      <c r="I37" s="21"/>
+      <c r="J37" s="21"/>
       <c r="K37" s="3" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="12">
+      <c r="A38" s="24">
         <v>43768</v>
       </c>
-      <c r="B38" s="13"/>
-      <c r="C38" s="13"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="14">
+      <c r="B38" s="12"/>
+      <c r="C38" s="12"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="13">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G38" s="13"/>
-      <c r="H38" s="13"/>
-      <c r="I38" s="13"/>
-      <c r="J38" s="14"/>
+      <c r="G38" s="12"/>
+      <c r="H38" s="12"/>
+      <c r="I38" s="12"/>
+      <c r="J38" s="13"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="12">
+      <c r="A39" s="24">
         <v>43769</v>
       </c>
-      <c r="B39" s="13"/>
-      <c r="C39" s="13"/>
-      <c r="D39" s="13"/>
-      <c r="E39" s="14">
+      <c r="B39" s="12"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="13">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G39" s="13"/>
-      <c r="H39" s="13"/>
-      <c r="I39" s="13"/>
-      <c r="J39" s="14"/>
+      <c r="G39" s="12"/>
+      <c r="H39" s="12"/>
+      <c r="I39" s="12"/>
+      <c r="J39" s="13"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E40" s="16"/>
-      <c r="J40" s="16"/>
+      <c r="E40" s="15"/>
+      <c r="J40" s="15"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E41" s="16"/>
-      <c r="J41" s="16"/>
+      <c r="E41" s="15"/>
+      <c r="J41" s="15"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
@@ -1581,19 +1593,19 @@
         <v>34</v>
       </c>
       <c r="D42" s="3">
-        <f>SUM(D4:D29)</f>
-        <v>41.5</v>
-      </c>
-      <c r="E42" s="16">
+        <f>SUM(D4:D30)</f>
+        <v>49.5</v>
+      </c>
+      <c r="E42" s="15">
         <f>SUM(E4:E37)</f>
-        <v>185.5</v>
+        <v>193.5</v>
       </c>
       <c r="I42" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="J42" s="16">
+      <c r="J42" s="15">
         <f>SUM(J4:J37)</f>
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed homepage navbar and added custom scroll bar and table css
</commit_message>
<xml_diff>
--- a/Documentation/Working Hours.xlsx
+++ b/Documentation/Working Hours.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="56">
   <si>
     <t>Working Hours</t>
   </si>
@@ -175,6 +175,18 @@
   </si>
   <si>
     <t>addStudent, database, deleteStudent</t>
+  </si>
+  <si>
+    <t>Fixed navbar in faculty login, removed navbar &amp; set content to center in main login page</t>
+  </si>
+  <si>
+    <t>shake effect and table</t>
+  </si>
+  <si>
+    <t>homepage navbar</t>
+  </si>
+  <si>
+    <t>fixed homepage navbar and custom scroll bar and table css</t>
   </si>
 </sst>
 </file>
@@ -183,7 +195,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-    <numFmt numFmtId="166" formatCode="[$-14009]dddd\,\ d\ mmmm\,\ yyyy;@"/>
+    <numFmt numFmtId="165" formatCode="[$-14009]dddd\,\ d\ mmmm\,\ yyyy;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -335,11 +347,11 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -624,8 +636,8 @@
   <dimension ref="A1:K42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="81" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J31" sqref="J31"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -637,7 +649,7 @@
     <col min="5" max="5" width="10.5703125" style="20" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="1.85546875" style="3" customWidth="1"/>
     <col min="7" max="7" width="64" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="82.140625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="87.140625" style="3" customWidth="1"/>
     <col min="9" max="9" width="46.28515625" style="3" customWidth="1"/>
     <col min="10" max="10" width="19.42578125" style="20" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.28515625" style="3" bestFit="1" customWidth="1"/>
@@ -648,20 +660,20 @@
       <c r="A1" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
+      <c r="B1" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
       <c r="E1" s="18" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="19"/>
-      <c r="G1" s="23" t="s">
+      <c r="G1" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
       <c r="J1" s="16" t="s">
         <v>7</v>
       </c>
@@ -713,7 +725,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="24">
+      <c r="A4" s="23">
         <v>43735</v>
       </c>
       <c r="B4" s="2">
@@ -741,7 +753,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="24">
+      <c r="A5" s="23">
         <v>43736</v>
       </c>
       <c r="B5" s="2">
@@ -769,7 +781,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="24">
+      <c r="A6" s="23">
         <v>43737</v>
       </c>
       <c r="B6" s="2">
@@ -797,7 +809,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="24">
+      <c r="A7" s="23">
         <v>43738</v>
       </c>
       <c r="B7" s="2">
@@ -824,7 +836,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="24"/>
+      <c r="A8" s="23"/>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
@@ -836,7 +848,7 @@
       <c r="J8" s="9"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="24">
+      <c r="A9" s="23">
         <v>43739</v>
       </c>
       <c r="B9" s="2">
@@ -864,7 +876,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="24">
+      <c r="A10" s="23">
         <v>43740</v>
       </c>
       <c r="B10" s="2">
@@ -894,7 +906,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="24">
+      <c r="A11" s="23">
         <v>43741</v>
       </c>
       <c r="B11" s="2">
@@ -924,7 +936,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="24">
+      <c r="A12" s="23">
         <v>43742</v>
       </c>
       <c r="B12" s="2">
@@ -954,7 +966,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="24">
+      <c r="A13" s="23">
         <v>43743</v>
       </c>
       <c r="B13" s="10">
@@ -982,7 +994,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="24">
+      <c r="A14" s="23">
         <v>43744</v>
       </c>
       <c r="B14" s="10">
@@ -1010,7 +1022,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="24">
+      <c r="A15" s="23">
         <v>43745</v>
       </c>
       <c r="B15" s="10">
@@ -1038,7 +1050,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="24">
+      <c r="A16" s="23">
         <v>43746</v>
       </c>
       <c r="B16" s="2">
@@ -1068,7 +1080,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="24">
+      <c r="A17" s="23">
         <v>43747</v>
       </c>
       <c r="B17" s="2">
@@ -1098,7 +1110,7 @@
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="24">
+      <c r="A18" s="23">
         <v>43748</v>
       </c>
       <c r="B18" s="2">
@@ -1124,7 +1136,7 @@
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="24">
+      <c r="A19" s="23">
         <v>43749</v>
       </c>
       <c r="B19" s="2">
@@ -1149,7 +1161,7 @@
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="24">
+      <c r="A20" s="23">
         <v>43750</v>
       </c>
       <c r="B20" s="2">
@@ -1175,7 +1187,7 @@
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="24">
+      <c r="A21" s="23">
         <v>43751</v>
       </c>
       <c r="B21" s="2">
@@ -1201,7 +1213,7 @@
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="24">
+      <c r="A22" s="23">
         <v>43752</v>
       </c>
       <c r="B22" s="2">
@@ -1225,7 +1237,7 @@
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="24">
+      <c r="A23" s="23">
         <v>43753</v>
       </c>
       <c r="B23" s="12">
@@ -1249,7 +1261,7 @@
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="24">
+      <c r="A24" s="23">
         <v>43754</v>
       </c>
       <c r="B24" s="12">
@@ -1273,7 +1285,7 @@
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="24">
+      <c r="A25" s="23">
         <v>43755</v>
       </c>
       <c r="B25" s="12">
@@ -1301,7 +1313,7 @@
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="24">
+      <c r="A26" s="23">
         <v>43756</v>
       </c>
       <c r="B26" s="12">
@@ -1325,7 +1337,7 @@
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="24">
+      <c r="A27" s="23">
         <v>43757</v>
       </c>
       <c r="B27" s="12">
@@ -1347,7 +1359,7 @@
       <c r="J27" s="13"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="24">
+      <c r="A28" s="23">
         <v>43758</v>
       </c>
       <c r="B28" s="12">
@@ -1373,7 +1385,7 @@
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="24">
+      <c r="A29" s="23">
         <v>43759</v>
       </c>
       <c r="B29" s="12"/>
@@ -1399,19 +1411,19 @@
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="24">
+      <c r="A30" s="23">
         <v>43760</v>
       </c>
       <c r="B30" s="12"/>
       <c r="C30" s="12">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D30" s="12">
         <v>5</v>
       </c>
       <c r="E30" s="13">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G30" s="12"/>
       <c r="H30" s="12" t="s">
@@ -1425,39 +1437,51 @@
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="24">
+      <c r="A31" s="23">
         <v>43761</v>
       </c>
       <c r="B31" s="12"/>
-      <c r="C31" s="12"/>
+      <c r="C31" s="12">
+        <v>5</v>
+      </c>
       <c r="D31" s="12"/>
       <c r="E31" s="13">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G31" s="12"/>
-      <c r="H31" s="12"/>
+      <c r="H31" s="12" t="s">
+        <v>52</v>
+      </c>
       <c r="I31" s="12"/>
-      <c r="J31" s="13"/>
+      <c r="J31" s="13">
+        <v>3</v>
+      </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="24">
+      <c r="A32" s="23">
         <v>43762</v>
       </c>
       <c r="B32" s="12"/>
-      <c r="C32" s="12"/>
+      <c r="C32" s="12">
+        <v>6.5</v>
+      </c>
       <c r="D32" s="12"/>
       <c r="E32" s="13">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>6.5</v>
       </c>
       <c r="G32" s="12"/>
-      <c r="H32" s="12"/>
+      <c r="H32" s="12" t="s">
+        <v>53</v>
+      </c>
       <c r="I32" s="12"/>
-      <c r="J32" s="13"/>
+      <c r="J32" s="13">
+        <v>1</v>
+      </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="24">
+      <c r="A33" s="23">
         <v>43763</v>
       </c>
       <c r="B33" s="12"/>
@@ -1473,39 +1497,51 @@
       <c r="J33" s="13"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="24">
+      <c r="A34" s="23">
         <v>43764</v>
       </c>
       <c r="B34" s="12"/>
-      <c r="C34" s="12"/>
+      <c r="C34" s="12">
+        <v>7</v>
+      </c>
       <c r="D34" s="12"/>
       <c r="E34" s="13">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G34" s="12"/>
-      <c r="H34" s="12"/>
+      <c r="H34" s="12" t="s">
+        <v>54</v>
+      </c>
       <c r="I34" s="12"/>
-      <c r="J34" s="13"/>
+      <c r="J34" s="13">
+        <v>1</v>
+      </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="24">
+      <c r="A35" s="23">
         <v>43765</v>
       </c>
       <c r="B35" s="12"/>
-      <c r="C35" s="12"/>
+      <c r="C35" s="12">
+        <v>5</v>
+      </c>
       <c r="D35" s="12"/>
       <c r="E35" s="13">
         <f t="shared" ref="E35" si="5">(B35+C35+D35)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G35" s="12"/>
-      <c r="H35" s="12"/>
+      <c r="H35" s="12" t="s">
+        <v>55</v>
+      </c>
       <c r="I35" s="12"/>
-      <c r="J35" s="13"/>
+      <c r="J35" s="13">
+        <v>3</v>
+      </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="24">
+      <c r="A36" s="23">
         <v>43766</v>
       </c>
       <c r="B36" s="12"/>
@@ -1521,7 +1557,7 @@
       <c r="J36" s="13"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="24">
+      <c r="A37" s="23">
         <v>43767</v>
       </c>
       <c r="B37" s="21"/>
@@ -1541,7 +1577,7 @@
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="24">
+      <c r="A38" s="23">
         <v>43768</v>
       </c>
       <c r="B38" s="12"/>
@@ -1557,7 +1593,7 @@
       <c r="J38" s="13"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="24">
+      <c r="A39" s="23">
         <v>43769</v>
       </c>
       <c r="B39" s="12"/>
@@ -1590,7 +1626,7 @@
       </c>
       <c r="C42" s="3">
         <f>SUM(C3:C37)</f>
-        <v>34</v>
+        <v>58.5</v>
       </c>
       <c r="D42" s="3">
         <f>SUM(D4:D30)</f>
@@ -1598,14 +1634,14 @@
       </c>
       <c r="E42" s="15">
         <f>SUM(E4:E37)</f>
-        <v>193.5</v>
+        <v>218</v>
       </c>
       <c r="I42" s="3" t="s">
         <v>21</v>
       </c>
       <c r="J42" s="15">
         <f>SUM(J4:J37)</f>
-        <v>60</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
i dont remember :P, look inside for changes
</commit_message>
<xml_diff>
--- a/Documentation/Working Hours.xlsx
+++ b/Documentation/Working Hours.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="73">
   <si>
     <t>Working Hours</t>
   </si>
@@ -190,17 +190,65 @@
   </si>
   <si>
     <t>Logo animation</t>
+  </si>
+  <si>
+    <t>soldering rpi keypad and fit inside box</t>
+  </si>
+  <si>
+    <t>performance tweeks, view subject , subject attendance</t>
+  </si>
+  <si>
+    <t>minimizer and profile pic upload</t>
+  </si>
+  <si>
+    <t>GUI, profile pic for students</t>
+  </si>
+  <si>
+    <t>preferences for combined timetable, disable on labs completed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bug fixes, add student, unselectable text, </t>
+  </si>
+  <si>
+    <t>fixed new week redundancy</t>
+  </si>
+  <si>
+    <t>time based timetable edit, fix date printing</t>
+  </si>
+  <si>
+    <t>convert full site to ajax</t>
+  </si>
+  <si>
+    <t>ajax bug fix</t>
+  </si>
+  <si>
+    <t>subject selection bugs, slot management</t>
+  </si>
+  <si>
+    <t>new gui, session management</t>
+  </si>
+  <si>
+    <t>gui bugs, data tables</t>
+  </si>
+  <si>
+    <t xml:space="preserve">save stud details , back button </t>
+  </si>
+  <si>
+    <t>subject batch for students, back button bug fix</t>
+  </si>
+  <si>
+    <t>save stud details</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
     <numFmt numFmtId="165" formatCode="[$-14009]dddd\,\ d\ mmmm\,\ yyyy;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -416,7 +464,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -451,7 +499,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -628,22 +676,22 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K45"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="81" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J42" sqref="J42"/>
+    <sheetView tabSelected="1" zoomScale="81" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H48" sqref="H48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="31.28515625" style="7" customWidth="1"/>
     <col min="2" max="2" width="9.28515625" style="3" bestFit="1" customWidth="1"/>
@@ -659,7 +707,7 @@
     <col min="12" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="30">
       <c r="A1" s="17" t="s">
         <v>5</v>
       </c>
@@ -681,7 +729,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2" s="1"/>
       <c r="B2" s="4" t="s">
         <v>1</v>
@@ -704,7 +752,7 @@
       </c>
       <c r="J2" s="13"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" s="11" t="s">
         <v>26</v>
       </c>
@@ -727,7 +775,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4" s="23">
         <v>43735</v>
       </c>
@@ -755,7 +803,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5" s="23">
         <v>43736</v>
       </c>
@@ -783,7 +831,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6" s="23">
         <v>43737</v>
       </c>
@@ -811,7 +859,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" s="8" customFormat="1">
       <c r="A7" s="23">
         <v>43738</v>
       </c>
@@ -838,7 +886,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="A8" s="23"/>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
@@ -850,7 +898,7 @@
       <c r="I8" s="9"/>
       <c r="J8" s="9"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="A9" s="23">
         <v>43739</v>
       </c>
@@ -878,7 +926,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10">
       <c r="A10" s="23">
         <v>43740</v>
       </c>
@@ -908,7 +956,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10">
       <c r="A11" s="23">
         <v>43741</v>
       </c>
@@ -938,7 +986,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10">
       <c r="A12" s="23">
         <v>43742</v>
       </c>
@@ -968,7 +1016,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10">
       <c r="A13" s="23">
         <v>43743</v>
       </c>
@@ -996,7 +1044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10">
       <c r="A14" s="23">
         <v>43744</v>
       </c>
@@ -1024,7 +1072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10">
       <c r="A15" s="23">
         <v>43745</v>
       </c>
@@ -1052,7 +1100,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10">
       <c r="A16" s="23">
         <v>43746</v>
       </c>
@@ -1082,7 +1130,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10">
       <c r="A17" s="23">
         <v>43747</v>
       </c>
@@ -1112,7 +1160,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10">
       <c r="A18" s="23">
         <v>43748</v>
       </c>
@@ -1138,7 +1186,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10">
       <c r="A19" s="23">
         <v>43749</v>
       </c>
@@ -1163,7 +1211,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10">
       <c r="A20" s="23">
         <v>43750</v>
       </c>
@@ -1189,7 +1237,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10">
       <c r="A21" s="23">
         <v>43751</v>
       </c>
@@ -1215,7 +1263,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10">
       <c r="A22" s="23">
         <v>43752</v>
       </c>
@@ -1239,7 +1287,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10">
       <c r="A23" s="23">
         <v>43753</v>
       </c>
@@ -1263,7 +1311,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10">
       <c r="A24" s="23">
         <v>43754</v>
       </c>
@@ -1287,7 +1335,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10">
       <c r="A25" s="23">
         <v>43755</v>
       </c>
@@ -1315,7 +1363,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10">
       <c r="A26" s="23">
         <v>43756</v>
       </c>
@@ -1339,7 +1387,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10">
       <c r="A27" s="23">
         <v>43757</v>
       </c>
@@ -1361,7 +1409,7 @@
       </c>
       <c r="J27" s="13"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10">
       <c r="A28" s="23">
         <v>43758</v>
       </c>
@@ -1387,7 +1435,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10">
       <c r="A29" s="23">
         <v>43759</v>
       </c>
@@ -1404,7 +1452,9 @@
         <f t="shared" si="2"/>
         <v>23.5</v>
       </c>
-      <c r="G29" s="12"/>
+      <c r="G29" s="12" t="s">
+        <v>58</v>
+      </c>
       <c r="H29" s="12" t="s">
         <v>48</v>
       </c>
@@ -1415,7 +1465,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10">
       <c r="A30" s="23">
         <v>43760</v>
       </c>
@@ -1432,7 +1482,9 @@
         <f t="shared" si="2"/>
         <v>19</v>
       </c>
-      <c r="G30" s="12"/>
+      <c r="G30" s="12" t="s">
+        <v>59</v>
+      </c>
       <c r="H30" s="12" t="s">
         <v>49</v>
       </c>
@@ -1443,7 +1495,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10">
       <c r="A31" s="23">
         <v>43761</v>
       </c>
@@ -1458,7 +1510,9 @@
         <f t="shared" si="2"/>
         <v>14</v>
       </c>
-      <c r="G31" s="12"/>
+      <c r="G31" s="12" t="s">
+        <v>60</v>
+      </c>
       <c r="H31" s="12" t="s">
         <v>52</v>
       </c>
@@ -1467,7 +1521,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10">
       <c r="A32" s="23">
         <v>43762</v>
       </c>
@@ -1482,7 +1536,9 @@
         <f t="shared" si="2"/>
         <v>17.5</v>
       </c>
-      <c r="G32" s="12"/>
+      <c r="G32" s="12" t="s">
+        <v>61</v>
+      </c>
       <c r="H32" s="12" t="s">
         <v>53</v>
       </c>
@@ -1491,7 +1547,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11">
       <c r="A33" s="23">
         <v>43763</v>
       </c>
@@ -1504,17 +1560,19 @@
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="G33" s="12"/>
+      <c r="G33" s="12" t="s">
+        <v>62</v>
+      </c>
       <c r="H33" s="12"/>
       <c r="I33" s="12"/>
       <c r="J33" s="13"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11">
       <c r="A34" s="23">
         <v>43764</v>
       </c>
       <c r="B34" s="12">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C34" s="12">
         <v>7</v>
@@ -1522,9 +1580,11 @@
       <c r="D34" s="12"/>
       <c r="E34" s="13">
         <f t="shared" si="2"/>
-        <v>7</v>
-      </c>
-      <c r="G34" s="12"/>
+        <v>12</v>
+      </c>
+      <c r="G34" s="12" t="s">
+        <v>63</v>
+      </c>
       <c r="H34" s="12" t="s">
         <v>54</v>
       </c>
@@ -1533,12 +1593,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11">
       <c r="A35" s="23">
         <v>43765</v>
       </c>
       <c r="B35" s="12">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C35" s="12">
         <v>5</v>
@@ -1546,7 +1606,7 @@
       <c r="D35" s="12"/>
       <c r="E35" s="13">
         <f t="shared" ref="E35" si="5">(B35+C35+D35)</f>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G35" s="12"/>
       <c r="H35" s="12" t="s">
@@ -1557,7 +1617,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11">
       <c r="A36" s="23">
         <v>43766</v>
       </c>
@@ -1570,26 +1630,30 @@
         <f t="shared" ref="E36" si="6">B36+C36+D36</f>
         <v>5</v>
       </c>
-      <c r="G36" s="12"/>
+      <c r="G36" s="12" t="s">
+        <v>64</v>
+      </c>
       <c r="H36" s="12"/>
       <c r="I36" s="12"/>
       <c r="J36" s="13"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11">
       <c r="A37" s="23">
         <v>43767</v>
       </c>
       <c r="B37" s="21">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C37" s="21"/>
       <c r="D37" s="21"/>
       <c r="E37" s="21">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="F37" s="22"/>
-      <c r="G37" s="21"/>
+      <c r="G37" s="12" t="s">
+        <v>65</v>
+      </c>
       <c r="H37" s="21"/>
       <c r="I37" s="21"/>
       <c r="J37" s="21"/>
@@ -1597,12 +1661,12 @@
         <v>47</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11">
       <c r="A38" s="23">
         <v>43768</v>
       </c>
       <c r="B38" s="12">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C38" s="12">
         <v>2</v>
@@ -1610,9 +1674,11 @@
       <c r="D38" s="12"/>
       <c r="E38" s="13">
         <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="G38" s="12"/>
+        <v>7</v>
+      </c>
+      <c r="G38" s="12" t="s">
+        <v>65</v>
+      </c>
       <c r="H38" s="12" t="s">
         <v>56</v>
       </c>
@@ -1621,7 +1687,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11">
       <c r="A39" s="23">
         <v>43769</v>
       </c>
@@ -1634,12 +1700,14 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G39" s="12"/>
+      <c r="G39" s="12" t="s">
+        <v>65</v>
+      </c>
       <c r="H39" s="12"/>
       <c r="I39" s="12"/>
       <c r="J39" s="13"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11">
       <c r="A40" s="7">
         <v>1</v>
       </c>
@@ -1647,9 +1715,12 @@
         <v>5</v>
       </c>
       <c r="E40" s="15"/>
+      <c r="G40" s="12" t="s">
+        <v>65</v>
+      </c>
       <c r="J40" s="15"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11">
       <c r="A41" s="7">
         <v>2</v>
       </c>
@@ -1657,9 +1728,12 @@
         <v>13</v>
       </c>
       <c r="E41" s="15"/>
+      <c r="G41" s="12" t="s">
+        <v>65</v>
+      </c>
       <c r="J41" s="15"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11">
       <c r="A42" s="7">
         <v>3</v>
       </c>
@@ -1667,6 +1741,9 @@
         <v>9</v>
       </c>
       <c r="E42" s="15"/>
+      <c r="G42" s="12" t="s">
+        <v>65</v>
+      </c>
       <c r="I42" s="3" t="s">
         <v>21</v>
       </c>
@@ -1675,13 +1752,13 @@
         <v>69</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11">
       <c r="A43" s="7" t="s">
         <v>20</v>
       </c>
       <c r="B43" s="3">
         <f>SUM(B3:B42)</f>
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="C43" s="3">
         <f t="shared" ref="C43:E43" si="7">SUM(C3:C42)</f>
@@ -1693,11 +1770,117 @@
       </c>
       <c r="E43" s="3">
         <f t="shared" si="7"/>
-        <v>297</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+      <c r="G43" s="12"/>
+    </row>
+    <row r="44" spans="1:11">
+      <c r="G44" s="12"/>
+    </row>
+    <row r="45" spans="1:11">
+      <c r="A45" s="7">
+        <v>4</v>
+      </c>
+      <c r="B45" s="3">
+        <v>6</v>
+      </c>
       <c r="E45" s="15"/>
+      <c r="G45" s="12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11">
+      <c r="A46" s="7">
+        <v>5</v>
+      </c>
+      <c r="B46" s="3">
+        <v>5</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11">
+      <c r="A47" s="7">
+        <v>6</v>
+      </c>
+      <c r="B47" s="3">
+        <v>9</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11">
+      <c r="A48" s="7">
+        <v>7</v>
+      </c>
+      <c r="B48" s="3">
+        <v>9</v>
+      </c>
+      <c r="G48" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="A49" s="7">
+        <v>8</v>
+      </c>
+      <c r="B49" s="3">
+        <v>7</v>
+      </c>
+      <c r="G49" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50" s="7">
+        <v>9</v>
+      </c>
+      <c r="B50" s="3">
+        <v>9</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="A51" s="7">
+        <v>10</v>
+      </c>
+      <c r="B51" s="3">
+        <v>5</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="A52" s="7">
+        <v>11</v>
+      </c>
+      <c r="B52" s="3">
+        <v>8</v>
+      </c>
+      <c r="G52" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
+      <c r="A53" s="7">
+        <v>12</v>
+      </c>
+      <c r="B53" s="3">
+        <v>5</v>
+      </c>
+      <c r="G53" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
+      <c r="A54" s="7">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
fixed resetpassword page and added css to editSlot
</commit_message>
<xml_diff>
--- a/Documentation/Working Hours.xlsx
+++ b/Documentation/Working Hours.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="96">
   <si>
     <t>Working Hours</t>
   </si>
@@ -304,6 +304,9 @@
   </si>
   <si>
     <t>background and dropdowns CSS</t>
+  </si>
+  <si>
+    <t>fixed resetpassword page and added css to editSlot</t>
   </si>
 </sst>
 </file>
@@ -809,8 +812,8 @@
   <dimension ref="A1:K61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D55" sqref="D55"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H58" sqref="H58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -821,8 +824,8 @@
     <col min="4" max="4" width="5.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.85546875" style="18" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="1.85546875" style="3" customWidth="1"/>
-    <col min="7" max="7" width="64" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="69.42578125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="64" style="3" customWidth="1"/>
+    <col min="8" max="8" width="75.7109375" style="3" customWidth="1"/>
     <col min="9" max="9" width="69.5703125" style="3" customWidth="1"/>
     <col min="10" max="10" width="19.42578125" style="18" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18.7109375" style="3" bestFit="1" customWidth="1"/>
@@ -1322,7 +1325,7 @@
         <v>3</v>
       </c>
       <c r="E18" s="13">
-        <f t="shared" ref="E18:E55" si="2">B18+C18+D18</f>
+        <f t="shared" ref="E18:E56" si="2">B18+C18+D18</f>
         <v>11</v>
       </c>
       <c r="G18" s="12" t="s">
@@ -1920,14 +1923,14 @@
         <v>5</v>
       </c>
       <c r="C38" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D38" s="12">
         <v>0</v>
       </c>
       <c r="E38" s="13">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G38" s="12" t="s">
         <v>62</v>
@@ -1939,7 +1942,7 @@
         <v>88</v>
       </c>
       <c r="J38" s="13">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
@@ -2444,6 +2447,29 @@
         <v>2</v>
       </c>
     </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56" s="11">
+        <v>43785</v>
+      </c>
+      <c r="B56" s="12"/>
+      <c r="C56" s="12">
+        <v>5</v>
+      </c>
+      <c r="D56" s="12"/>
+      <c r="E56" s="13">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="F56" s="12"/>
+      <c r="G56" s="12"/>
+      <c r="H56" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="I56" s="12"/>
+      <c r="J56" s="13">
+        <v>2</v>
+      </c>
+    </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
         <v>19</v>
@@ -2453,8 +2479,8 @@
         <v>279</v>
       </c>
       <c r="C61" s="12">
-        <f>SUM(C3:C55)</f>
-        <v>71</v>
+        <f>SUM(C3:C56)</f>
+        <v>78</v>
       </c>
       <c r="D61" s="12">
         <f>SUM(D3:D54)</f>
@@ -2462,14 +2488,14 @@
       </c>
       <c r="E61" s="13">
         <f>SUM(E3:E54)</f>
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="I61" s="12" t="s">
         <v>20</v>
       </c>
       <c r="J61" s="20">
-        <f>SUM(J3:J55)</f>
-        <v>125</v>
+        <f>SUM(J3:J56)</f>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -2482,12 +2508,12 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3:D55">
+  <conditionalFormatting sqref="B3:D56">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3:I55">
+  <conditionalFormatting sqref="G3:I56">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"-"</formula>
     </cfRule>

</xml_diff>

<commit_message>
About us Page, hover in login page and editStudDetails javascript
</commit_message>
<xml_diff>
--- a/Documentation/Working Hours.xlsx
+++ b/Documentation/Working Hours.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="98">
   <si>
     <t>Working Hours</t>
   </si>
@@ -307,6 +307,12 @@
   </si>
   <si>
     <t>fixed resetpassword page and added css to editSlot</t>
+  </si>
+  <si>
+    <t>About us page</t>
+  </si>
+  <si>
+    <t>About us Page, hover in login page and editStudDetails javascipt</t>
   </si>
 </sst>
 </file>
@@ -809,11 +815,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K61"/>
+  <dimension ref="A1:K74"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H58" sqref="H58"/>
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J70" sqref="J70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1325,7 +1331,7 @@
         <v>3</v>
       </c>
       <c r="E18" s="13">
-        <f t="shared" ref="E18:E56" si="2">B18+C18+D18</f>
+        <f t="shared" ref="E18:E73" si="2">B18+C18+D18</f>
         <v>11</v>
       </c>
       <c r="G18" s="12" t="s">
@@ -2470,32 +2476,334 @@
         <v>2</v>
       </c>
     </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57" s="11">
+        <v>43786</v>
+      </c>
+      <c r="B57" s="12"/>
+      <c r="C57" s="12"/>
+      <c r="D57" s="12"/>
+      <c r="E57" s="13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F57" s="12"/>
+      <c r="G57" s="12"/>
+      <c r="H57" s="12"/>
+      <c r="I57" s="12"/>
+      <c r="J57" s="13"/>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58" s="11">
+        <v>43787</v>
+      </c>
+      <c r="B58" s="12"/>
+      <c r="C58" s="12"/>
+      <c r="D58" s="12"/>
+      <c r="E58" s="13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F58" s="12"/>
+      <c r="G58" s="12"/>
+      <c r="H58" s="12"/>
+      <c r="I58" s="12"/>
+      <c r="J58" s="13"/>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59" s="11">
+        <v>43788</v>
+      </c>
+      <c r="B59" s="12"/>
+      <c r="C59" s="12"/>
+      <c r="D59" s="12"/>
+      <c r="E59" s="13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F59" s="12"/>
+      <c r="G59" s="12"/>
+      <c r="H59" s="12"/>
+      <c r="I59" s="12"/>
+      <c r="J59" s="13"/>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A60" s="11">
+        <v>43789</v>
+      </c>
+      <c r="B60" s="12"/>
+      <c r="C60" s="12"/>
+      <c r="D60" s="12"/>
+      <c r="E60" s="13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F60" s="12"/>
+      <c r="G60" s="12"/>
+      <c r="H60" s="12"/>
+      <c r="I60" s="12"/>
+      <c r="J60" s="13"/>
+    </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A61" s="7" t="s">
+      <c r="A61" s="11">
+        <v>43790</v>
+      </c>
+      <c r="B61" s="12"/>
+      <c r="C61" s="12"/>
+      <c r="D61" s="12"/>
+      <c r="E61" s="13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F61" s="12"/>
+      <c r="G61" s="12"/>
+      <c r="H61" s="12"/>
+      <c r="I61" s="12"/>
+      <c r="J61" s="13"/>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A62" s="11">
+        <v>43791</v>
+      </c>
+      <c r="B62" s="12"/>
+      <c r="C62" s="12"/>
+      <c r="D62" s="12"/>
+      <c r="E62" s="13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F62" s="12"/>
+      <c r="G62" s="12"/>
+      <c r="H62" s="12"/>
+      <c r="I62" s="12"/>
+      <c r="J62" s="13"/>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A63" s="11">
+        <v>43792</v>
+      </c>
+      <c r="B63" s="12"/>
+      <c r="C63" s="12"/>
+      <c r="D63" s="12"/>
+      <c r="E63" s="13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F63" s="12"/>
+      <c r="G63" s="12"/>
+      <c r="H63" s="12"/>
+      <c r="I63" s="12"/>
+      <c r="J63" s="13"/>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A64" s="11">
+        <v>43793</v>
+      </c>
+      <c r="B64" s="12"/>
+      <c r="C64" s="12"/>
+      <c r="D64" s="12"/>
+      <c r="E64" s="13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F64" s="12"/>
+      <c r="G64" s="12"/>
+      <c r="H64" s="12"/>
+      <c r="I64" s="12"/>
+      <c r="J64" s="13"/>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A65" s="11">
+        <v>43794</v>
+      </c>
+      <c r="B65" s="12"/>
+      <c r="C65" s="12"/>
+      <c r="D65" s="12"/>
+      <c r="E65" s="13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F65" s="12"/>
+      <c r="G65" s="12"/>
+      <c r="H65" s="12"/>
+      <c r="I65" s="12"/>
+      <c r="J65" s="13"/>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A66" s="11">
+        <v>43795</v>
+      </c>
+      <c r="B66" s="12"/>
+      <c r="C66" s="12"/>
+      <c r="D66" s="12"/>
+      <c r="E66" s="13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F66" s="12"/>
+      <c r="G66" s="12"/>
+      <c r="H66" s="12"/>
+      <c r="I66" s="12"/>
+      <c r="J66" s="13"/>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A67" s="11">
+        <v>43796</v>
+      </c>
+      <c r="B67" s="12"/>
+      <c r="C67" s="12"/>
+      <c r="D67" s="12"/>
+      <c r="E67" s="13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F67" s="12"/>
+      <c r="G67" s="12"/>
+      <c r="H67" s="12"/>
+      <c r="I67" s="12"/>
+      <c r="J67" s="13"/>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A68" s="11">
+        <v>43797</v>
+      </c>
+      <c r="B68" s="12"/>
+      <c r="C68" s="12"/>
+      <c r="D68" s="12"/>
+      <c r="E68" s="13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F68" s="12"/>
+      <c r="G68" s="12"/>
+      <c r="H68" s="12"/>
+      <c r="I68" s="12"/>
+      <c r="J68" s="13"/>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A69" s="11">
+        <v>43798</v>
+      </c>
+      <c r="B69" s="12"/>
+      <c r="C69" s="12"/>
+      <c r="D69" s="12"/>
+      <c r="E69" s="13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F69" s="12"/>
+      <c r="G69" s="12"/>
+      <c r="H69" s="12"/>
+      <c r="I69" s="12"/>
+      <c r="J69" s="13"/>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A70" s="11">
+        <v>43799</v>
+      </c>
+      <c r="B70" s="12"/>
+      <c r="C70" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="D70" s="12"/>
+      <c r="E70" s="13">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+      <c r="F70" s="12"/>
+      <c r="G70" s="12"/>
+      <c r="H70" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="I70" s="12"/>
+      <c r="J70" s="13"/>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A71" s="11">
+        <v>43800</v>
+      </c>
+      <c r="B71" s="12"/>
+      <c r="C71" s="12"/>
+      <c r="D71" s="12"/>
+      <c r="E71" s="13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F71" s="12"/>
+      <c r="G71" s="12"/>
+      <c r="H71" s="12"/>
+      <c r="I71" s="12"/>
+      <c r="J71" s="13"/>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A72" s="11">
+        <v>43801</v>
+      </c>
+      <c r="B72" s="12"/>
+      <c r="C72" s="12">
+        <v>5</v>
+      </c>
+      <c r="D72" s="12"/>
+      <c r="E72" s="13">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="F72" s="12"/>
+      <c r="G72" s="12"/>
+      <c r="H72" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="I72" s="12"/>
+      <c r="J72" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A73" s="11">
+        <v>43802</v>
+      </c>
+      <c r="B73" s="12"/>
+      <c r="C73" s="12"/>
+      <c r="D73" s="12"/>
+      <c r="E73" s="13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F73" s="12"/>
+      <c r="G73" s="12"/>
+      <c r="H73" s="12"/>
+      <c r="I73" s="12"/>
+      <c r="J73" s="13"/>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A74" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B61" s="12">
-        <f>SUM(B4:B54)</f>
+      <c r="B74" s="12">
+        <f>SUM(B4:B73)</f>
         <v>279</v>
       </c>
-      <c r="C61" s="12">
-        <f>SUM(C3:C56)</f>
-        <v>78</v>
-      </c>
-      <c r="D61" s="12">
-        <f>SUM(D3:D54)</f>
-        <v>121</v>
-      </c>
-      <c r="E61" s="13">
-        <f>SUM(E3:E54)</f>
-        <v>471</v>
-      </c>
-      <c r="I61" s="12" t="s">
+      <c r="C74" s="12">
+        <f>SUM(C3:C73)</f>
+        <v>83.5</v>
+      </c>
+      <c r="D74" s="12">
+        <f>SUM(D3:D73)</f>
+        <v>124</v>
+      </c>
+      <c r="E74" s="13">
+        <f>SUM(E3:E73)</f>
+        <v>486.5</v>
+      </c>
+      <c r="F74" s="12"/>
+      <c r="G74" s="12"/>
+      <c r="H74" s="12"/>
+      <c r="I74" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="J61" s="20">
-        <f>SUM(J3:J56)</f>
-        <v>128</v>
+      <c r="J74" s="20">
+        <f>SUM(J3:J73)</f>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -2503,17 +2811,17 @@
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="G1:I1"/>
   </mergeCells>
-  <conditionalFormatting sqref="I46">
+  <conditionalFormatting sqref="I46 B66:D73">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3:D56">
+  <conditionalFormatting sqref="B3:D65">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3:I56">
+  <conditionalFormatting sqref="G3:I56 G57:H74 I57:I73">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"-"</formula>
     </cfRule>

</xml_diff>

<commit_message>
About us page and tilt effect in login page
</commit_message>
<xml_diff>
--- a/Documentation/Working Hours.xlsx
+++ b/Documentation/Working Hours.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="100">
   <si>
     <t>Working Hours</t>
   </si>
@@ -316,6 +316,9 @@
   </si>
   <si>
     <t>editStudDetails javascipt and About us page</t>
+  </si>
+  <si>
+    <t>About us page and tilt effect in login page</t>
   </si>
 </sst>
 </file>
@@ -421,7 +424,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -515,6 +518,9 @@
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -591,7 +597,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -626,7 +632,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -811,11 +817,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K79"/>
+  <dimension ref="A1:K82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J75" sqref="J75"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G82" sqref="G82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1327,7 +1333,7 @@
         <v>3</v>
       </c>
       <c r="E18" s="13">
-        <f t="shared" ref="E18:E73" si="2">B18+C18+D18</f>
+        <f t="shared" ref="E18:E78" si="2">B18+C18+D18</f>
         <v>11</v>
       </c>
       <c r="G18" s="12" t="s">
@@ -2814,15 +2820,100 @@
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A74" s="11">
+        <v>43803</v>
+      </c>
+      <c r="B74" s="12"/>
+      <c r="C74" s="12"/>
+      <c r="D74" s="12"/>
+      <c r="E74" s="13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F74" s="12"/>
       <c r="G74" s="12"/>
       <c r="H74" s="12"/>
-      <c r="I74" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="J74" s="20">
-        <f>SUM(J3:J73)</f>
-        <v>132</v>
+      <c r="I74" s="12"/>
+      <c r="J74" s="13"/>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A75" s="11">
+        <v>43804</v>
+      </c>
+      <c r="B75" s="12"/>
+      <c r="C75" s="12"/>
+      <c r="D75" s="12"/>
+      <c r="E75" s="13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F75" s="12"/>
+      <c r="G75" s="12"/>
+      <c r="H75" s="12"/>
+      <c r="I75" s="12"/>
+      <c r="J75" s="13"/>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="11">
+        <v>43805</v>
+      </c>
+      <c r="B76" s="12"/>
+      <c r="C76" s="12"/>
+      <c r="D76" s="12"/>
+      <c r="E76" s="13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F76" s="12"/>
+      <c r="G76" s="12"/>
+      <c r="H76" s="12"/>
+      <c r="I76" s="12"/>
+      <c r="J76" s="13"/>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="11">
+        <v>43806</v>
+      </c>
+      <c r="B77" s="12"/>
+      <c r="C77" s="12">
+        <v>7</v>
+      </c>
+      <c r="D77" s="12"/>
+      <c r="E77" s="13">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="F77" s="12"/>
+      <c r="G77" s="12"/>
+      <c r="H77" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="I77" s="12"/>
+      <c r="J77" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="11">
+        <v>43807</v>
+      </c>
+      <c r="B78" s="12"/>
+      <c r="C78" s="12">
+        <v>4</v>
+      </c>
+      <c r="D78" s="12"/>
+      <c r="E78" s="13">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="F78" s="12"/>
+      <c r="G78" s="12"/>
+      <c r="H78" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="I78" s="12"/>
+      <c r="J78" s="13">
+        <v>2</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
@@ -2830,20 +2921,39 @@
         <v>19</v>
       </c>
       <c r="B79" s="12">
-        <f>SUM(B4:B73)</f>
+        <f>SUM(B4:B78)</f>
         <v>289</v>
       </c>
       <c r="C79" s="12">
-        <f>SUM(C3:C73)</f>
-        <v>86.5</v>
+        <f>SUM(C3:C78)</f>
+        <v>97.5</v>
       </c>
       <c r="D79" s="12">
-        <f>SUM(D3:D73)</f>
+        <f>SUM(D3:D78)</f>
         <v>124</v>
       </c>
       <c r="E79" s="13">
-        <f>SUM(E3:E73)</f>
-        <v>499.5</v>
+        <f>SUM(E3:E78)</f>
+        <v>510.5</v>
+      </c>
+      <c r="I79" s="12"/>
+      <c r="J79" s="32"/>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I80" s="12"/>
+      <c r="J80" s="32"/>
+    </row>
+    <row r="81" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I81" s="12"/>
+      <c r="J81" s="32"/>
+    </row>
+    <row r="82" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I82" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="J82" s="20">
+        <f>SUM(J3:J78)</f>
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -2851,12 +2961,12 @@
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="G1:I1"/>
   </mergeCells>
-  <conditionalFormatting sqref="I46 B3:D73">
+  <conditionalFormatting sqref="I46 B3:D78">
     <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3:I56 G57:H74 I57:I73">
+  <conditionalFormatting sqref="G3:I56 I57:I73 G57:H78">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"-"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Removed interactivity from particles.js and Fixed scrollbar in Aboutus page
</commit_message>
<xml_diff>
--- a/Documentation/Working Hours.xlsx
+++ b/Documentation/Working Hours.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="103">
   <si>
     <t>Working Hours</t>
   </si>
@@ -319,6 +319,15 @@
   </si>
   <si>
     <t>About us page and tilt effect in login page</t>
+  </si>
+  <si>
+    <t>Removed interactivity from particles.js and Fixed scrollbar in Aboutus page</t>
+  </si>
+  <si>
+    <t>Fixed logo in About us page and javascript in editStudDetails servlet</t>
+  </si>
+  <si>
+    <t>Fixed CSS and javascript in editStudDetails servle</t>
   </si>
 </sst>
 </file>
@@ -424,7 +433,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -518,9 +527,6 @@
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -817,11 +823,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K82"/>
+  <dimension ref="A1:K88"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G82" sqref="G82"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I81" sqref="I81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1333,7 +1339,7 @@
         <v>3</v>
       </c>
       <c r="E18" s="13">
-        <f t="shared" ref="E18:E78" si="2">B18+C18+D18</f>
+        <f t="shared" ref="E18:E81" si="2">B18+C18+D18</f>
         <v>11</v>
       </c>
       <c r="G18" s="12" t="s">
@@ -2917,43 +2923,202 @@
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A79" s="7" t="s">
+      <c r="A79" s="11">
+        <v>43808</v>
+      </c>
+      <c r="B79" s="12"/>
+      <c r="C79" s="12"/>
+      <c r="D79" s="12"/>
+      <c r="E79" s="13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F79" s="12"/>
+      <c r="G79" s="12"/>
+      <c r="H79" s="12"/>
+      <c r="I79" s="12"/>
+      <c r="J79" s="13"/>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="11">
+        <v>43809</v>
+      </c>
+      <c r="B80" s="12"/>
+      <c r="C80" s="12"/>
+      <c r="D80" s="12"/>
+      <c r="E80" s="13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F80" s="12"/>
+      <c r="G80" s="12"/>
+      <c r="H80" s="12"/>
+      <c r="I80" s="12"/>
+      <c r="J80" s="13"/>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="11">
+        <v>43810</v>
+      </c>
+      <c r="B81" s="12"/>
+      <c r="C81" s="12">
+        <v>4.5</v>
+      </c>
+      <c r="D81" s="12"/>
+      <c r="E81" s="13">
+        <f t="shared" si="2"/>
+        <v>4.5</v>
+      </c>
+      <c r="F81" s="12"/>
+      <c r="G81" s="12"/>
+      <c r="H81" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="I81" s="12"/>
+      <c r="J81" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="11">
+        <v>43811</v>
+      </c>
+      <c r="B82" s="12"/>
+      <c r="C82" s="12">
+        <v>5.5</v>
+      </c>
+      <c r="D82" s="12"/>
+      <c r="E82" s="13">
+        <f t="shared" ref="E82:E87" si="7">B82+C82+D82</f>
+        <v>5.5</v>
+      </c>
+      <c r="F82" s="12"/>
+      <c r="G82" s="12"/>
+      <c r="H82" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="I82" s="12"/>
+      <c r="J82" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="11">
+        <v>43812</v>
+      </c>
+      <c r="B83" s="12"/>
+      <c r="C83" s="12"/>
+      <c r="D83" s="12"/>
+      <c r="E83" s="13">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="F83" s="12"/>
+      <c r="G83" s="12"/>
+      <c r="H83" s="12"/>
+      <c r="I83" s="12"/>
+      <c r="J83" s="13"/>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="11">
+        <v>43813</v>
+      </c>
+      <c r="B84" s="12"/>
+      <c r="C84" s="12">
+        <v>1</v>
+      </c>
+      <c r="D84" s="12"/>
+      <c r="E84" s="13">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="F84" s="12"/>
+      <c r="G84" s="12"/>
+      <c r="H84" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="I84" s="12"/>
+      <c r="J84" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="11">
+        <v>43814</v>
+      </c>
+      <c r="B85" s="12"/>
+      <c r="C85" s="12"/>
+      <c r="D85" s="12"/>
+      <c r="E85" s="13">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="F85" s="12"/>
+      <c r="G85" s="12"/>
+      <c r="H85" s="12"/>
+      <c r="I85" s="12"/>
+      <c r="J85" s="13"/>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="11">
+        <v>43815</v>
+      </c>
+      <c r="B86" s="12"/>
+      <c r="C86" s="12"/>
+      <c r="D86" s="12"/>
+      <c r="E86" s="13">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="F86" s="12"/>
+      <c r="G86" s="12"/>
+      <c r="H86" s="12"/>
+      <c r="I86" s="12"/>
+      <c r="J86" s="13"/>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" s="11">
+        <v>43816</v>
+      </c>
+      <c r="B87" s="12"/>
+      <c r="C87" s="12"/>
+      <c r="D87" s="12"/>
+      <c r="E87" s="13">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="F87" s="12"/>
+      <c r="G87" s="12"/>
+      <c r="H87" s="12"/>
+      <c r="I87" s="12"/>
+      <c r="J87" s="13"/>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B79" s="12">
-        <f>SUM(B4:B78)</f>
+      <c r="B88" s="12">
+        <f>SUM(B4:B87)</f>
         <v>289</v>
       </c>
-      <c r="C79" s="12">
-        <f>SUM(C3:C78)</f>
-        <v>97.5</v>
-      </c>
-      <c r="D79" s="12">
-        <f>SUM(D3:D78)</f>
+      <c r="C88" s="12">
+        <f>SUM(C3:C87)</f>
+        <v>108.5</v>
+      </c>
+      <c r="D88" s="12">
+        <f>SUM(D3:D87)</f>
         <v>124</v>
       </c>
-      <c r="E79" s="13">
-        <f>SUM(E3:E78)</f>
-        <v>510.5</v>
-      </c>
-      <c r="I79" s="12"/>
-      <c r="J79" s="32"/>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I80" s="12"/>
-      <c r="J80" s="32"/>
-    </row>
-    <row r="81" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I81" s="12"/>
-      <c r="J81" s="32"/>
-    </row>
-    <row r="82" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I82" s="12" t="s">
+      <c r="E88" s="13">
+        <f>SUM(E3:E87)</f>
+        <v>521.5</v>
+      </c>
+      <c r="I88" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="J82" s="20">
-        <f>SUM(J3:J78)</f>
-        <v>135</v>
+      <c r="J88" s="20">
+        <f>SUM(J3:J87)</f>
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -2961,12 +3126,12 @@
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="G1:I1"/>
   </mergeCells>
-  <conditionalFormatting sqref="I46 B3:D78">
+  <conditionalFormatting sqref="I46 B3:D87">
     <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3:I56 I57:I73 G57:H78">
+  <conditionalFormatting sqref="G3:I56 I57:I73 G57:H87">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"-"</formula>
     </cfRule>

</xml_diff>

<commit_message>
minor bugs, edit attendance
</commit_message>
<xml_diff>
--- a/Documentation/Working Hours.xlsx
+++ b/Documentation/Working Hours.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -333,12 +333,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
     <numFmt numFmtId="165" formatCode="[$-14009]dddd\,\ d\ mmmm\,\ yyyy;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -603,7 +603,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -638,7 +638,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -815,22 +815,22 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I81" sqref="I81"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H80" sqref="H80"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="31.28515625" style="7" customWidth="1"/>
     <col min="2" max="2" width="9.28515625" style="3" bestFit="1" customWidth="1"/>
@@ -846,7 +846,7 @@
     <col min="12" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="30">
       <c r="A1" s="15" t="s">
         <v>4</v>
       </c>
@@ -868,7 +868,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2" s="1"/>
       <c r="B2" s="4" t="s">
         <v>1</v>
@@ -891,7 +891,7 @@
       </c>
       <c r="J2" s="13"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" s="11" t="s">
         <v>25</v>
       </c>
@@ -918,7 +918,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4" s="19">
         <v>43735</v>
       </c>
@@ -948,7 +948,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5" s="19">
         <v>43736</v>
       </c>
@@ -978,7 +978,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6" s="19">
         <v>43737</v>
       </c>
@@ -1008,7 +1008,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" s="8" customFormat="1">
       <c r="A7" s="19">
         <v>43738</v>
       </c>
@@ -1039,7 +1039,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="A8" s="19"/>
       <c r="B8" s="9" t="s">
         <v>12</v>
@@ -1057,7 +1057,7 @@
       <c r="I8" s="9"/>
       <c r="J8" s="9"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="A9" s="19">
         <v>43739</v>
       </c>
@@ -1085,7 +1085,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10">
       <c r="A10" s="19">
         <v>43740</v>
       </c>
@@ -1115,7 +1115,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10">
       <c r="A11" s="19">
         <v>43741</v>
       </c>
@@ -1145,7 +1145,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10">
       <c r="A12" s="19">
         <v>43742</v>
       </c>
@@ -1175,7 +1175,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10">
       <c r="A13" s="19">
         <v>43743</v>
       </c>
@@ -1205,7 +1205,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10">
       <c r="A14" s="19">
         <v>43744</v>
       </c>
@@ -1235,7 +1235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10">
       <c r="A15" s="19">
         <v>43745</v>
       </c>
@@ -1265,7 +1265,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10">
       <c r="A16" s="19">
         <v>43746</v>
       </c>
@@ -1295,7 +1295,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10">
       <c r="A17" s="19">
         <v>43747</v>
       </c>
@@ -1325,7 +1325,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10">
       <c r="A18" s="19">
         <v>43748</v>
       </c>
@@ -1355,7 +1355,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10">
       <c r="A19" s="19">
         <v>43749</v>
       </c>
@@ -1385,7 +1385,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10">
       <c r="A20" s="19">
         <v>43750</v>
       </c>
@@ -1415,7 +1415,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10">
       <c r="A21" s="19">
         <v>43751</v>
       </c>
@@ -1445,7 +1445,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10">
       <c r="A22" s="19">
         <v>43752</v>
       </c>
@@ -1475,7 +1475,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10">
       <c r="A23" s="19">
         <v>43753</v>
       </c>
@@ -1505,7 +1505,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10">
       <c r="A24" s="19">
         <v>43754</v>
       </c>
@@ -1535,7 +1535,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" ht="30" customHeight="1">
       <c r="A25" s="27">
         <v>43755</v>
       </c>
@@ -1566,7 +1566,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10">
       <c r="A26" s="19">
         <v>43756</v>
       </c>
@@ -1596,7 +1596,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10">
       <c r="A27" s="19">
         <v>43757</v>
       </c>
@@ -1624,7 +1624,7 @@
       </c>
       <c r="J27" s="13"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10">
       <c r="A28" s="19">
         <v>43758</v>
       </c>
@@ -1654,7 +1654,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10">
       <c r="A29" s="19">
         <v>43759</v>
       </c>
@@ -1684,7 +1684,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10">
       <c r="A30" s="19">
         <v>43760</v>
       </c>
@@ -1714,7 +1714,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" ht="29.25" customHeight="1">
       <c r="A31" s="27">
         <v>43761</v>
       </c>
@@ -1745,7 +1745,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10">
       <c r="A32" s="19">
         <v>43762</v>
       </c>
@@ -1775,7 +1775,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11">
       <c r="A33" s="19">
         <v>43763</v>
       </c>
@@ -1805,7 +1805,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11">
       <c r="A34" s="19">
         <v>43764</v>
       </c>
@@ -1835,7 +1835,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11">
       <c r="A35" s="19">
         <v>43765</v>
       </c>
@@ -1865,7 +1865,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11">
       <c r="A36" s="19">
         <v>43766</v>
       </c>
@@ -1895,7 +1895,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11">
       <c r="A37" s="19">
         <v>43767</v>
       </c>
@@ -1929,7 +1929,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11">
       <c r="A38" s="19">
         <v>43768</v>
       </c>
@@ -1959,7 +1959,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11">
       <c r="A39" s="19">
         <v>43769</v>
       </c>
@@ -1987,7 +1987,7 @@
       </c>
       <c r="J39" s="13"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11">
       <c r="B40" s="21" t="s">
         <v>12</v>
       </c>
@@ -2004,7 +2004,7 @@
       <c r="I40" s="21"/>
       <c r="J40" s="21"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11">
       <c r="A41" s="11">
         <v>43770</v>
       </c>
@@ -2033,7 +2033,7 @@
       </c>
       <c r="J41" s="13"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11">
       <c r="A42" s="11">
         <v>43771</v>
       </c>
@@ -2062,7 +2062,7 @@
       </c>
       <c r="J42" s="13"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11">
       <c r="A43" s="11">
         <v>43772</v>
       </c>
@@ -2093,7 +2093,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11">
       <c r="A44" s="11">
         <v>43773</v>
       </c>
@@ -2124,7 +2124,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11">
       <c r="A45" s="11">
         <v>43774</v>
       </c>
@@ -2155,7 +2155,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11">
       <c r="A46" s="11">
         <v>43775</v>
       </c>
@@ -2186,7 +2186,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11">
       <c r="A47" s="11">
         <v>43776</v>
       </c>
@@ -2217,7 +2217,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11">
       <c r="A48" s="11">
         <v>43777</v>
       </c>
@@ -2248,7 +2248,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10">
       <c r="A49" s="11">
         <v>43778</v>
       </c>
@@ -2279,7 +2279,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10">
       <c r="A50" s="11">
         <v>43779</v>
       </c>
@@ -2308,7 +2308,7 @@
       </c>
       <c r="J50" s="13"/>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10">
       <c r="A51" s="11">
         <v>43780</v>
       </c>
@@ -2339,7 +2339,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10">
       <c r="A52" s="11">
         <v>43781</v>
       </c>
@@ -2370,7 +2370,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10">
       <c r="A53" s="11">
         <v>43782</v>
       </c>
@@ -2401,7 +2401,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10">
       <c r="A54" s="11">
         <v>43783</v>
       </c>
@@ -2430,7 +2430,7 @@
       </c>
       <c r="J54" s="13"/>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10">
       <c r="A55" s="11">
         <v>43784</v>
       </c>
@@ -2461,7 +2461,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10">
       <c r="A56" s="11">
         <v>43785</v>
       </c>
@@ -2486,7 +2486,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10">
       <c r="A57" s="11">
         <v>43786</v>
       </c>
@@ -2505,7 +2505,7 @@
       <c r="I57" s="12"/>
       <c r="J57" s="13"/>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10">
       <c r="A58" s="11">
         <v>43787</v>
       </c>
@@ -2524,7 +2524,7 @@
       <c r="I58" s="12"/>
       <c r="J58" s="13"/>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10">
       <c r="A59" s="11">
         <v>43788</v>
       </c>
@@ -2543,7 +2543,7 @@
       <c r="I59" s="12"/>
       <c r="J59" s="13"/>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10">
       <c r="A60" s="11">
         <v>43789</v>
       </c>
@@ -2562,7 +2562,7 @@
       <c r="I60" s="12"/>
       <c r="J60" s="13"/>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10">
       <c r="A61" s="11">
         <v>43790</v>
       </c>
@@ -2581,7 +2581,7 @@
       <c r="I61" s="12"/>
       <c r="J61" s="13"/>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10">
       <c r="A62" s="11">
         <v>43791</v>
       </c>
@@ -2600,7 +2600,7 @@
       <c r="I62" s="12"/>
       <c r="J62" s="13"/>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10">
       <c r="A63" s="11">
         <v>43792</v>
       </c>
@@ -2619,7 +2619,7 @@
       <c r="I63" s="12"/>
       <c r="J63" s="13"/>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10">
       <c r="A64" s="11">
         <v>43793</v>
       </c>
@@ -2638,7 +2638,7 @@
       <c r="I64" s="12"/>
       <c r="J64" s="13"/>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10">
       <c r="A65" s="11">
         <v>43794</v>
       </c>
@@ -2657,7 +2657,7 @@
       <c r="I65" s="12"/>
       <c r="J65" s="13"/>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10">
       <c r="A66" s="11">
         <v>43795</v>
       </c>
@@ -2676,7 +2676,7 @@
       <c r="I66" s="12"/>
       <c r="J66" s="13"/>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10">
       <c r="A67" s="11">
         <v>43796</v>
       </c>
@@ -2695,7 +2695,7 @@
       <c r="I67" s="12"/>
       <c r="J67" s="13"/>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10">
       <c r="A68" s="11">
         <v>43797</v>
       </c>
@@ -2714,7 +2714,7 @@
       <c r="I68" s="12"/>
       <c r="J68" s="13"/>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10">
       <c r="A69" s="11">
         <v>43798</v>
       </c>
@@ -2733,7 +2733,7 @@
       <c r="I69" s="12"/>
       <c r="J69" s="13"/>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10">
       <c r="A70" s="11">
         <v>43799</v>
       </c>
@@ -2756,7 +2756,7 @@
       <c r="I70" s="12"/>
       <c r="J70" s="13"/>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10">
       <c r="A71" s="11">
         <v>43800</v>
       </c>
@@ -2775,7 +2775,7 @@
       <c r="I71" s="12"/>
       <c r="J71" s="13"/>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10">
       <c r="A72" s="11">
         <v>43801</v>
       </c>
@@ -2800,7 +2800,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10">
       <c r="A73" s="11">
         <v>43802</v>
       </c>
@@ -2825,16 +2825,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10">
       <c r="A74" s="11">
         <v>43803</v>
       </c>
-      <c r="B74" s="12"/>
+      <c r="B74" s="12">
+        <v>2</v>
+      </c>
       <c r="C74" s="12"/>
       <c r="D74" s="12"/>
       <c r="E74" s="13">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F74" s="12"/>
       <c r="G74" s="12"/>
@@ -2842,11 +2844,13 @@
       <c r="I74" s="12"/>
       <c r="J74" s="13"/>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10">
       <c r="A75" s="11">
         <v>43804</v>
       </c>
-      <c r="B75" s="12"/>
+      <c r="B75" s="12">
+        <v>0</v>
+      </c>
       <c r="C75" s="12"/>
       <c r="D75" s="12"/>
       <c r="E75" s="13">
@@ -2859,11 +2863,13 @@
       <c r="I75" s="12"/>
       <c r="J75" s="13"/>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10">
       <c r="A76" s="11">
         <v>43805</v>
       </c>
-      <c r="B76" s="12"/>
+      <c r="B76" s="12">
+        <v>0</v>
+      </c>
       <c r="C76" s="12"/>
       <c r="D76" s="12"/>
       <c r="E76" s="13">
@@ -2876,18 +2882,20 @@
       <c r="I76" s="12"/>
       <c r="J76" s="13"/>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10">
       <c r="A77" s="11">
         <v>43806</v>
       </c>
-      <c r="B77" s="12"/>
+      <c r="B77" s="12">
+        <v>1</v>
+      </c>
       <c r="C77" s="12">
         <v>7</v>
       </c>
       <c r="D77" s="12"/>
       <c r="E77" s="13">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F77" s="12"/>
       <c r="G77" s="12"/>
@@ -2899,11 +2907,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10">
       <c r="A78" s="11">
         <v>43807</v>
       </c>
-      <c r="B78" s="12"/>
+      <c r="B78" s="12">
+        <v>0</v>
+      </c>
       <c r="C78" s="12">
         <v>4</v>
       </c>
@@ -2922,11 +2932,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10">
       <c r="A79" s="11">
         <v>43808</v>
       </c>
-      <c r="B79" s="12"/>
+      <c r="B79" s="12">
+        <v>0</v>
+      </c>
       <c r="C79" s="12"/>
       <c r="D79" s="12"/>
       <c r="E79" s="13">
@@ -2939,16 +2951,18 @@
       <c r="I79" s="12"/>
       <c r="J79" s="13"/>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10">
       <c r="A80" s="11">
         <v>43809</v>
       </c>
-      <c r="B80" s="12"/>
+      <c r="B80" s="12">
+        <v>3</v>
+      </c>
       <c r="C80" s="12"/>
       <c r="D80" s="12"/>
       <c r="E80" s="13">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F80" s="12"/>
       <c r="G80" s="12"/>
@@ -2956,11 +2970,13 @@
       <c r="I80" s="12"/>
       <c r="J80" s="13"/>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10">
       <c r="A81" s="11">
         <v>43810</v>
       </c>
-      <c r="B81" s="12"/>
+      <c r="B81" s="12">
+        <v>0</v>
+      </c>
       <c r="C81" s="12">
         <v>4.5</v>
       </c>
@@ -2979,18 +2995,20 @@
         <v>2</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10">
       <c r="A82" s="11">
         <v>43811</v>
       </c>
-      <c r="B82" s="12"/>
+      <c r="B82" s="12">
+        <v>12</v>
+      </c>
       <c r="C82" s="12">
         <v>5.5</v>
       </c>
       <c r="D82" s="12"/>
       <c r="E82" s="13">
         <f t="shared" ref="E82:E87" si="7">B82+C82+D82</f>
-        <v>5.5</v>
+        <v>17.5</v>
       </c>
       <c r="F82" s="12"/>
       <c r="G82" s="12"/>
@@ -3002,16 +3020,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10">
       <c r="A83" s="11">
         <v>43812</v>
       </c>
-      <c r="B83" s="12"/>
+      <c r="B83" s="12">
+        <v>10</v>
+      </c>
       <c r="C83" s="12"/>
       <c r="D83" s="12"/>
       <c r="E83" s="13">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F83" s="12"/>
       <c r="G83" s="12"/>
@@ -3019,18 +3039,20 @@
       <c r="I83" s="12"/>
       <c r="J83" s="13"/>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10">
       <c r="A84" s="11">
         <v>43813</v>
       </c>
-      <c r="B84" s="12"/>
+      <c r="B84" s="12">
+        <v>13</v>
+      </c>
       <c r="C84" s="12">
         <v>1</v>
       </c>
       <c r="D84" s="12"/>
       <c r="E84" s="13">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F84" s="12"/>
       <c r="G84" s="12"/>
@@ -3042,16 +3064,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10">
       <c r="A85" s="11">
         <v>43814</v>
       </c>
-      <c r="B85" s="12"/>
+      <c r="B85" s="12">
+        <v>14</v>
+      </c>
       <c r="C85" s="12"/>
       <c r="D85" s="12"/>
       <c r="E85" s="13">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="F85" s="12"/>
       <c r="G85" s="12"/>
@@ -3059,7 +3083,7 @@
       <c r="I85" s="12"/>
       <c r="J85" s="13"/>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10">
       <c r="A86" s="11">
         <v>43815</v>
       </c>
@@ -3076,7 +3100,7 @@
       <c r="I86" s="12"/>
       <c r="J86" s="13"/>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10">
       <c r="A87" s="11">
         <v>43816</v>
       </c>
@@ -3093,13 +3117,13 @@
       <c r="I87" s="12"/>
       <c r="J87" s="13"/>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10">
       <c r="A88" s="7" t="s">
         <v>19</v>
       </c>
       <c r="B88" s="12">
         <f>SUM(B4:B87)</f>
-        <v>289</v>
+        <v>344</v>
       </c>
       <c r="C88" s="12">
         <f>SUM(C3:C87)</f>
@@ -3111,7 +3135,7 @@
       </c>
       <c r="E88" s="13">
         <f>SUM(E3:E87)</f>
-        <v>521.5</v>
+        <v>576.5</v>
       </c>
       <c r="I88" s="12" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
Minor changes in attendance servlet
</commit_message>
<xml_diff>
--- a/Documentation/Working Hours.xlsx
+++ b/Documentation/Working Hours.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
-  <workbookPr filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="162913"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="112">
   <si>
     <t>Working Hours</t>
   </si>
@@ -349,17 +349,23 @@
   </si>
   <si>
     <t>BIMAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validation text in editAddStudent &amp; editDelStudent Servlets and validations in addSubject &amp; addFaculty Servlets </t>
+  </si>
+  <si>
+    <t>attendance servlet</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
     <numFmt numFmtId="165" formatCode="[$-14009]dddd\,\ d\ mmmm\,\ yyyy;@"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -571,9 +577,6 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="8" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -586,54 +589,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="1" builtinId="10"/>
   </cellStyles>
-  <dxfs count="14">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="8">
     <dxf>
       <fill>
         <patternFill>
@@ -958,22 +922,22 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K96"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G91" sqref="G91"/>
+      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H88" sqref="H88"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.28515625" style="5" customWidth="1"/>
     <col min="2" max="2" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
@@ -982,36 +946,36 @@
     <col min="5" max="5" width="15.85546875" style="14" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="1.85546875" style="1" customWidth="1"/>
     <col min="7" max="7" width="64" style="1" customWidth="1"/>
-    <col min="8" max="8" width="75.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="104.42578125" style="1" customWidth="1"/>
     <col min="9" max="9" width="69.5703125" style="1" customWidth="1"/>
     <col min="10" max="10" width="19.42578125" style="14" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="30">
+    <row r="1" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="28" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
+      <c r="B1" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
       <c r="E1" s="12" t="s">
         <v>93</v>
       </c>
       <c r="F1" s="13"/>
-      <c r="G1" s="28" t="s">
+      <c r="G1" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
       <c r="J1" s="11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
       <c r="B2" s="2" t="s">
         <v>1</v>
@@ -1034,7 +998,7 @@
       </c>
       <c r="J2" s="10"/>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>25</v>
       </c>
@@ -1061,7 +1025,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="15">
         <v>43735</v>
       </c>
@@ -1091,7 +1055,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="15">
         <v>43736</v>
       </c>
@@ -1121,7 +1085,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="15">
         <v>43737</v>
       </c>
@@ -1151,7 +1115,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="6" customFormat="1">
+    <row r="7" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="15">
         <v>43738</v>
       </c>
@@ -1182,7 +1146,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="15"/>
       <c r="B8" s="7" t="s">
         <v>12</v>
@@ -1200,7 +1164,7 @@
       <c r="I8" s="7"/>
       <c r="J8" s="7"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="15">
         <v>43739</v>
       </c>
@@ -1228,7 +1192,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="15">
         <v>43740</v>
       </c>
@@ -1258,7 +1222,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="15">
         <v>43741</v>
       </c>
@@ -1288,7 +1252,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="15">
         <v>43742</v>
       </c>
@@ -1318,7 +1282,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="15">
         <v>43743</v>
       </c>
@@ -1348,7 +1312,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="15">
         <v>43744</v>
       </c>
@@ -1378,7 +1342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="15">
         <v>43745</v>
       </c>
@@ -1408,7 +1372,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="15">
         <v>43746</v>
       </c>
@@ -1438,7 +1402,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="15">
         <v>43747</v>
       </c>
@@ -1468,7 +1432,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="15">
         <v>43748</v>
       </c>
@@ -1498,7 +1462,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="15">
         <v>43749</v>
       </c>
@@ -1528,7 +1492,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="15">
         <v>43750</v>
       </c>
@@ -1558,7 +1522,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="15">
         <v>43751</v>
       </c>
@@ -1588,7 +1552,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="15">
         <v>43752</v>
       </c>
@@ -1618,7 +1582,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="15">
         <v>43753</v>
       </c>
@@ -1648,7 +1612,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="15">
         <v>43754</v>
       </c>
@@ -1678,7 +1642,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="30" customHeight="1">
+    <row r="25" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="23">
         <v>43755</v>
       </c>
@@ -1709,7 +1673,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="15">
         <v>43756</v>
       </c>
@@ -1739,7 +1703,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="15">
         <v>43757</v>
       </c>
@@ -1767,7 +1731,7 @@
       </c>
       <c r="J27" s="10"/>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="15">
         <v>43758</v>
       </c>
@@ -1797,7 +1761,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="15">
         <v>43759</v>
       </c>
@@ -1827,7 +1791,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="15">
         <v>43760</v>
       </c>
@@ -1857,7 +1821,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="29.25" customHeight="1">
+    <row r="31" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="23">
         <v>43761</v>
       </c>
@@ -1888,7 +1852,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="15">
         <v>43762</v>
       </c>
@@ -1918,7 +1882,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:11">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="15">
         <v>43763</v>
       </c>
@@ -1948,7 +1912,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:11">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="15">
         <v>43764</v>
       </c>
@@ -1978,7 +1942,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:11">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="15">
         <v>43765</v>
       </c>
@@ -2008,7 +1972,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:11">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="15">
         <v>43766</v>
       </c>
@@ -2038,7 +2002,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:11">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="15">
         <v>43767</v>
       </c>
@@ -2072,7 +2036,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="38" spans="1:11">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="15">
         <v>43768</v>
       </c>
@@ -2102,7 +2066,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:11">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="15">
         <v>43769</v>
       </c>
@@ -2130,7 +2094,7 @@
       </c>
       <c r="J39" s="10"/>
     </row>
-    <row r="40" spans="1:11">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B40" s="17" t="s">
         <v>12</v>
       </c>
@@ -2147,7 +2111,7 @@
       <c r="I40" s="17"/>
       <c r="J40" s="17"/>
     </row>
-    <row r="41" spans="1:11">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="8">
         <v>43770</v>
       </c>
@@ -2176,7 +2140,7 @@
       </c>
       <c r="J41" s="10"/>
     </row>
-    <row r="42" spans="1:11">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="8">
         <v>43771</v>
       </c>
@@ -2205,7 +2169,7 @@
       </c>
       <c r="J42" s="10"/>
     </row>
-    <row r="43" spans="1:11">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="8">
         <v>43772</v>
       </c>
@@ -2236,7 +2200,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:11">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="8">
         <v>43773</v>
       </c>
@@ -2267,7 +2231,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:11">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="8">
         <v>43774</v>
       </c>
@@ -2298,7 +2262,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:11">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="8">
         <v>43775</v>
       </c>
@@ -2329,7 +2293,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:11">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="8">
         <v>43776</v>
       </c>
@@ -2360,7 +2324,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:11">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="8">
         <v>43777</v>
       </c>
@@ -2391,7 +2355,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="8">
         <v>43778</v>
       </c>
@@ -2422,7 +2386,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="8">
         <v>43779</v>
       </c>
@@ -2451,7 +2415,7 @@
       </c>
       <c r="J50" s="10"/>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="8">
         <v>43780</v>
       </c>
@@ -2482,7 +2446,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="8">
         <v>43781</v>
       </c>
@@ -2513,7 +2477,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:10">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="8">
         <v>43782</v>
       </c>
@@ -2544,7 +2508,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:10">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="8">
         <v>43783</v>
       </c>
@@ -2573,7 +2537,7 @@
       </c>
       <c r="J54" s="10"/>
     </row>
-    <row r="55" spans="1:10">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="8">
         <v>43784</v>
       </c>
@@ -2604,7 +2568,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:10">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="8">
         <v>43785</v>
       </c>
@@ -2629,7 +2593,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:10">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="8">
         <v>43786</v>
       </c>
@@ -2648,7 +2612,7 @@
       <c r="I57" s="9"/>
       <c r="J57" s="10"/>
     </row>
-    <row r="58" spans="1:10">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="8">
         <v>43787</v>
       </c>
@@ -2667,7 +2631,7 @@
       <c r="I58" s="9"/>
       <c r="J58" s="10"/>
     </row>
-    <row r="59" spans="1:10">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="8">
         <v>43788</v>
       </c>
@@ -2686,7 +2650,7 @@
       <c r="I59" s="9"/>
       <c r="J59" s="10"/>
     </row>
-    <row r="60" spans="1:10">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="8">
         <v>43789</v>
       </c>
@@ -2707,7 +2671,7 @@
       </c>
       <c r="J60" s="10"/>
     </row>
-    <row r="61" spans="1:10">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="8">
         <v>43790</v>
       </c>
@@ -2728,7 +2692,7 @@
       </c>
       <c r="J61" s="10"/>
     </row>
-    <row r="62" spans="1:10">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="8">
         <v>43791</v>
       </c>
@@ -2749,7 +2713,7 @@
       </c>
       <c r="J62" s="10"/>
     </row>
-    <row r="63" spans="1:10">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="8">
         <v>43792</v>
       </c>
@@ -2770,7 +2734,7 @@
       </c>
       <c r="J63" s="10"/>
     </row>
-    <row r="64" spans="1:10">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="8">
         <v>43793</v>
       </c>
@@ -2791,7 +2755,7 @@
       </c>
       <c r="J64" s="10"/>
     </row>
-    <row r="65" spans="1:10">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="8">
         <v>43794</v>
       </c>
@@ -2812,7 +2776,7 @@
       </c>
       <c r="J65" s="10"/>
     </row>
-    <row r="66" spans="1:10">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="8">
         <v>43795</v>
       </c>
@@ -2833,7 +2797,7 @@
       </c>
       <c r="J66" s="10"/>
     </row>
-    <row r="67" spans="1:10">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="8">
         <v>43796</v>
       </c>
@@ -2854,7 +2818,7 @@
       </c>
       <c r="J67" s="10"/>
     </row>
-    <row r="68" spans="1:10">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="8">
         <v>43797</v>
       </c>
@@ -2873,7 +2837,7 @@
       <c r="I68" s="9"/>
       <c r="J68" s="10"/>
     </row>
-    <row r="69" spans="1:10">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="8">
         <v>43798</v>
       </c>
@@ -2892,7 +2856,7 @@
       <c r="I69" s="9"/>
       <c r="J69" s="10"/>
     </row>
-    <row r="70" spans="1:10">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="8">
         <v>43799</v>
       </c>
@@ -2915,19 +2879,19 @@
       <c r="I70" s="9"/>
       <c r="J70" s="10"/>
     </row>
-    <row r="71" spans="1:10">
-      <c r="A71" s="29"/>
-      <c r="B71" s="30"/>
-      <c r="C71" s="30"/>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A71" s="28"/>
+      <c r="B71" s="29"/>
+      <c r="C71" s="29"/>
       <c r="D71" s="9"/>
-      <c r="E71" s="30"/>
-      <c r="F71" s="30"/>
-      <c r="G71" s="30"/>
-      <c r="H71" s="30"/>
-      <c r="I71" s="30"/>
-      <c r="J71" s="30"/>
-    </row>
-    <row r="72" spans="1:10">
+      <c r="E71" s="29"/>
+      <c r="F71" s="29"/>
+      <c r="G71" s="29"/>
+      <c r="H71" s="29"/>
+      <c r="I71" s="29"/>
+      <c r="J71" s="29"/>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="8">
         <v>43800</v>
       </c>
@@ -2946,7 +2910,7 @@
       <c r="I72" s="9"/>
       <c r="J72" s="10"/>
     </row>
-    <row r="73" spans="1:10">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="8">
         <v>43801</v>
       </c>
@@ -2973,7 +2937,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="74" spans="1:10">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="8">
         <v>43802</v>
       </c>
@@ -3000,7 +2964,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:10">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="8">
         <v>43803</v>
       </c>
@@ -3019,7 +2983,7 @@
       <c r="I75" s="9"/>
       <c r="J75" s="10"/>
     </row>
-    <row r="76" spans="1:10">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="8">
         <v>43804</v>
       </c>
@@ -3040,7 +3004,7 @@
       </c>
       <c r="J76" s="10"/>
     </row>
-    <row r="77" spans="1:10">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="8">
         <v>43805</v>
       </c>
@@ -3061,7 +3025,7 @@
       </c>
       <c r="J77" s="10"/>
     </row>
-    <row r="78" spans="1:10">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="8">
         <v>43806</v>
       </c>
@@ -3088,7 +3052,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:10">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="8">
         <v>43807</v>
       </c>
@@ -3115,7 +3079,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="80" spans="1:10">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="8">
         <v>43808</v>
       </c>
@@ -3131,12 +3095,12 @@
       <c r="F80" s="9"/>
       <c r="G80" s="9"/>
       <c r="H80" s="9"/>
-      <c r="I80" s="31" t="s">
+      <c r="I80" s="30" t="s">
         <v>109</v>
       </c>
       <c r="J80" s="10"/>
     </row>
-    <row r="81" spans="1:10">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="8">
         <v>43809</v>
       </c>
@@ -3152,12 +3116,12 @@
       <c r="F81" s="9"/>
       <c r="G81" s="9"/>
       <c r="H81" s="9"/>
-      <c r="I81" s="31" t="s">
+      <c r="I81" s="30" t="s">
         <v>109</v>
       </c>
       <c r="J81" s="10"/>
     </row>
-    <row r="82" spans="1:10">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="8">
         <v>43810</v>
       </c>
@@ -3177,12 +3141,12 @@
       <c r="H82" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="I82" s="31" t="s">
+      <c r="I82" s="30" t="s">
         <v>109</v>
       </c>
       <c r="J82" s="10"/>
     </row>
-    <row r="83" spans="1:10">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="8">
         <v>43811</v>
       </c>
@@ -3202,12 +3166,12 @@
       <c r="H83" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="I83" s="31" t="s">
+      <c r="I83" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="J83" s="32"/>
-    </row>
-    <row r="84" spans="1:10">
+      <c r="J83" s="31"/>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="8">
         <v>43812</v>
       </c>
@@ -3223,12 +3187,12 @@
       <c r="F84" s="9"/>
       <c r="G84" s="9"/>
       <c r="H84" s="9"/>
-      <c r="I84" s="31" t="s">
+      <c r="I84" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="J84" s="32"/>
-    </row>
-    <row r="85" spans="1:10">
+      <c r="J84" s="31"/>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="8">
         <v>43813</v>
       </c>
@@ -3248,146 +3212,160 @@
       <c r="H85" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="I85" s="31" t="s">
+      <c r="I85" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="J85" s="32"/>
-    </row>
-    <row r="86" spans="1:10">
+      <c r="J85" s="31"/>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="8">
         <v>43814</v>
       </c>
       <c r="B86" s="9">
         <v>14</v>
       </c>
-      <c r="C86" s="9"/>
+      <c r="C86" s="9">
+        <v>4.5</v>
+      </c>
       <c r="D86" s="9"/>
       <c r="E86" s="10">
         <f t="shared" si="7"/>
-        <v>14</v>
+        <v>18.5</v>
       </c>
       <c r="F86" s="9"/>
       <c r="G86" s="9"/>
-      <c r="H86" s="9"/>
+      <c r="H86" s="9" t="s">
+        <v>110</v>
+      </c>
       <c r="I86" s="9"/>
-      <c r="J86" s="32"/>
-    </row>
-    <row r="87" spans="1:10">
+      <c r="J86" s="31">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="8">
         <v>43815</v>
       </c>
       <c r="B87" s="9"/>
-      <c r="C87" s="9"/>
+      <c r="C87" s="9">
+        <v>1</v>
+      </c>
       <c r="D87" s="9"/>
-      <c r="E87" s="32">
+      <c r="E87" s="31">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F87" s="9"/>
       <c r="G87" s="9"/>
-      <c r="H87" s="9"/>
+      <c r="H87" s="9" t="s">
+        <v>111</v>
+      </c>
       <c r="I87" s="9"/>
-      <c r="J87" s="32"/>
-    </row>
-    <row r="88" spans="1:10">
+      <c r="J87" s="31"/>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="8">
         <v>43816</v>
       </c>
       <c r="B88" s="9"/>
-      <c r="C88" s="9"/>
+      <c r="C88" s="9">
+        <v>5</v>
+      </c>
       <c r="D88" s="9"/>
-      <c r="E88" s="32"/>
+      <c r="E88" s="31"/>
       <c r="F88" s="9"/>
       <c r="G88" s="9"/>
-      <c r="H88" s="9"/>
+      <c r="H88" s="9" t="s">
+        <v>111</v>
+      </c>
       <c r="I88" s="9"/>
-      <c r="J88" s="32"/>
-    </row>
-    <row r="89" spans="1:10">
+      <c r="J88" s="31"/>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="8">
         <v>43817</v>
       </c>
       <c r="B89" s="9"/>
       <c r="C89" s="9"/>
       <c r="D89" s="9"/>
-      <c r="E89" s="32"/>
+      <c r="E89" s="31"/>
       <c r="F89" s="9"/>
       <c r="G89" s="9"/>
       <c r="H89" s="9"/>
       <c r="I89" s="9"/>
-      <c r="J89" s="32"/>
-    </row>
-    <row r="90" spans="1:10">
+      <c r="J89" s="31"/>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="8">
         <v>43818</v>
       </c>
       <c r="B90" s="9"/>
       <c r="C90" s="9"/>
       <c r="D90" s="9"/>
-      <c r="E90" s="32"/>
+      <c r="E90" s="31"/>
       <c r="F90" s="9"/>
       <c r="G90" s="9"/>
       <c r="H90" s="9"/>
       <c r="I90" s="9"/>
-      <c r="J90" s="32"/>
-    </row>
-    <row r="91" spans="1:10">
+      <c r="J90" s="31"/>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="8">
         <v>43819</v>
       </c>
       <c r="B91" s="9"/>
       <c r="C91" s="9"/>
       <c r="D91" s="9"/>
-      <c r="E91" s="32"/>
+      <c r="E91" s="31"/>
       <c r="F91" s="9"/>
       <c r="G91" s="9"/>
       <c r="H91" s="9"/>
       <c r="I91" s="9"/>
-      <c r="J91" s="32"/>
-    </row>
-    <row r="92" spans="1:10">
+      <c r="J91" s="31"/>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="8">
         <v>43820</v>
       </c>
       <c r="B92" s="9"/>
       <c r="C92" s="9"/>
       <c r="D92" s="9"/>
-      <c r="E92" s="32"/>
+      <c r="E92" s="31"/>
       <c r="F92" s="9"/>
       <c r="G92" s="9"/>
       <c r="H92" s="9"/>
       <c r="I92" s="9"/>
-      <c r="J92" s="32"/>
-    </row>
-    <row r="93" spans="1:10">
+      <c r="J92" s="31"/>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="8">
         <v>43821</v>
       </c>
       <c r="B93" s="9"/>
       <c r="C93" s="9"/>
       <c r="D93" s="9"/>
-      <c r="E93" s="32"/>
+      <c r="E93" s="31"/>
       <c r="F93" s="9"/>
       <c r="G93" s="9"/>
       <c r="H93" s="9"/>
       <c r="I93" s="9"/>
-      <c r="J93" s="32"/>
-    </row>
-    <row r="94" spans="1:10">
+      <c r="J93" s="31"/>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="8">
         <v>43822</v>
       </c>
       <c r="B94" s="9"/>
       <c r="C94" s="9"/>
       <c r="D94" s="9"/>
-      <c r="E94" s="32"/>
+      <c r="E94" s="31"/>
       <c r="F94" s="9"/>
       <c r="G94" s="9"/>
       <c r="H94" s="9"/>
       <c r="I94" s="9"/>
-      <c r="J94" s="32"/>
-    </row>
-    <row r="96" spans="1:10">
+      <c r="J94" s="31"/>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
         <v>19</v>
       </c>
@@ -3397,22 +3375,22 @@
       </c>
       <c r="C96" s="9">
         <f>SUM(C3:C94)</f>
-        <v>108.5</v>
+        <v>119</v>
       </c>
       <c r="D96" s="9">
         <f>SUM(D3:D94)</f>
         <v>134</v>
       </c>
       <c r="E96" s="10">
-        <f>SUM(E3:E79)</f>
-        <v>524.5</v>
+        <f>SUM(E3:E94)</f>
+        <v>609</v>
       </c>
       <c r="I96" s="9" t="s">
         <v>20</v>
       </c>
       <c r="J96" s="16">
-        <f>SUM(J3:J79)</f>
-        <v>135</v>
+        <f>SUM(J3:J94)</f>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -3421,42 +3399,42 @@
     <mergeCell ref="G1:I1"/>
   </mergeCells>
   <conditionalFormatting sqref="I46 B3:D87">
-    <cfRule type="cellIs" dxfId="13" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:I56 I57:I73 G57:H87">
-    <cfRule type="cellIs" dxfId="12" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I46 B3:D56 B80:B86 B57:C79 D57:D86">
-    <cfRule type="cellIs" dxfId="11" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:I56 I57:I74 G57:H79">
-    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B75:B86">
-    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C80:C86">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H80:H90">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H75:H85">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>